<commit_message>
completed all questions except for 8-bonus and 9
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick Nash\Documents\nss-data-analytics-08\projects\budget_lookups-thenicknash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208F161E-6A2D-4915-82A5-AEE86247F6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8804C4EB-7279-4350-B9DE-E9425C37250D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
   <si>
     <t>Department</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>test functions</t>
   </si>
 </sst>
 </file>
@@ -813,7 +816,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -825,6 +828,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1182,16 +1187,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="15.85546875" customWidth="1"/>
@@ -1268,8 +1275,8 @@
         <f>IFERROR(D2 / B2, 0)</f>
         <v>-4.3170750765267295E-2</v>
       </c>
-      <c r="F2">
-        <f>_xlfn.RANK.EQ(E2, E:E,0)</f>
+      <c r="F2" s="9">
+        <f>_xlfn.RANK.EQ($E2, $E$2:$E$52) +COUNTIF(E$2:E2,E2) -1</f>
         <v>38</v>
       </c>
       <c r="G2">
@@ -1286,8 +1293,8 @@
         <f>IFERROR(I2 / G2, 0)</f>
         <v>-9.4972027086493035E-2</v>
       </c>
-      <c r="K2">
-        <f>_xlfn.RANK.EQ(J2, J:J,0)</f>
+      <c r="K2" s="10">
+        <f>_xlfn.RANK.EQ($J2, $J$2:$J$52) +COUNTIF(J$2:J2,J2) -1</f>
         <v>42</v>
       </c>
       <c r="L2">
@@ -1304,8 +1311,8 @@
         <f>IFERROR(N2/L2, 0)</f>
         <v>-5.6484362894991494E-2</v>
       </c>
-      <c r="P2">
-        <f>_xlfn.RANK.EQ(O2,O:O,0)</f>
+      <c r="P2" s="10">
+        <f>_xlfn.RANK.EQ($O2, $O$2:$O$52) +COUNTIF(O$2:O2,O2) -1</f>
         <v>38</v>
       </c>
     </row>
@@ -1327,8 +1334,8 @@
         <f t="shared" ref="E3:E52" si="1">IFERROR(D3 / B3, 0)</f>
         <v>-2.3069981751824741E-2</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F52" si="2">_xlfn.RANK.EQ(E3, E:E,0)</f>
+      <c r="F3" s="9">
+        <f>_xlfn.RANK.EQ($E3, $E$2:$E$52) +COUNTIF(E$2:E3,E3) -1</f>
         <v>30</v>
       </c>
       <c r="G3">
@@ -1338,15 +1345,15 @@
         <v>312433.70999999897</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I52" si="3">H3-G3</f>
+        <f t="shared" ref="I3:I52" si="2">H3-G3</f>
         <v>-22366.290000001027</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J52" si="4">IFERROR(I3 / G3, 0)</f>
+        <f t="shared" ref="J3:J52" si="3">IFERROR(I3 / G3, 0)</f>
         <v>-6.6804928315415249E-2</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">_xlfn.RANK.EQ(J3, J:J,0)</f>
+      <c r="K3" s="10">
+        <f>_xlfn.RANK.EQ($J3, $J$2:$J$52) +COUNTIF(J$2:J3,J3) -1</f>
         <v>38</v>
       </c>
       <c r="L3">
@@ -1356,15 +1363,15 @@
         <v>322263.03999999998</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N52" si="6">M3-L3</f>
+        <f t="shared" ref="N3:N52" si="4">M3-L3</f>
         <v>-436.96000000002095</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O52" si="7">IFERROR(N3/L3, 0)</f>
+        <f t="shared" ref="O3:O52" si="5">IFERROR(N3/L3, 0)</f>
         <v>-1.3540749922529313E-3</v>
       </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P52" si="8">_xlfn.RANK.EQ(O3,O:O,0)</f>
+      <c r="P3" s="10">
+        <f>_xlfn.RANK.EQ($O3, $O$2:$O$52) +COUNTIF(O$2:O3,O3) -1</f>
         <v>15</v>
       </c>
     </row>
@@ -1386,8 +1393,8 @@
         <f t="shared" si="1"/>
         <v>-4.9327413275443007E-3</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="2"/>
+      <c r="F4" s="9">
+        <f>_xlfn.RANK.EQ($E4, $E$2:$E$52) +COUNTIF(E$2:E4,E4) -1</f>
         <v>10</v>
       </c>
       <c r="G4">
@@ -1397,15 +1404,15 @@
         <v>3589693.2099999902</v>
       </c>
       <c r="I4">
+        <f t="shared" si="2"/>
+        <v>-62606.790000009816</v>
+      </c>
+      <c r="J4" s="5">
         <f t="shared" si="3"/>
-        <v>-62606.790000009816</v>
-      </c>
-      <c r="J4" s="5">
-        <f t="shared" si="4"/>
         <v>-1.7141743558856015E-2</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="5"/>
+      <c r="K4" s="10">
+        <f>_xlfn.RANK.EQ($J4, $J$2:$J$52) +COUNTIF(J$2:J4,J4) -1</f>
         <v>16</v>
       </c>
       <c r="L4">
@@ -1415,15 +1422,15 @@
         <v>3564983.04999999</v>
       </c>
       <c r="N4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-97416.950000009965</v>
       </c>
       <c r="O4" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.6599210899959033E-2</v>
       </c>
-      <c r="P4">
-        <f t="shared" si="8"/>
+      <c r="P4" s="10">
+        <f>_xlfn.RANK.EQ($O4, $O$2:$O$52) +COUNTIF(O$2:O4,O4) -1</f>
         <v>27</v>
       </c>
     </row>
@@ -1445,8 +1452,8 @@
         <f t="shared" si="1"/>
         <v>-9.4273968477453174E-2</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
+      <c r="F5" s="9">
+        <f>_xlfn.RANK.EQ($E5, $E$2:$E$52) +COUNTIF(E$2:E5,E5) -1</f>
         <v>48</v>
       </c>
       <c r="G5">
@@ -1456,15 +1463,15 @@
         <v>7020609.3200000003</v>
       </c>
       <c r="I5">
+        <f t="shared" si="2"/>
+        <v>-947690.6799999997</v>
+      </c>
+      <c r="J5" s="5">
         <f t="shared" si="3"/>
-        <v>-947690.6799999997</v>
-      </c>
-      <c r="J5" s="5">
-        <f t="shared" si="4"/>
         <v>-0.118932605449092</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="5"/>
+      <c r="K5" s="10">
+        <f>_xlfn.RANK.EQ($J5, $J$2:$J$52) +COUNTIF(J$2:J5,J5) -1</f>
         <v>47</v>
       </c>
       <c r="L5">
@@ -1474,15 +1481,15 @@
         <v>7497322.9100000001</v>
       </c>
       <c r="N5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-262277.08999999985</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-3.3800336357544182E-2</v>
       </c>
-      <c r="P5">
-        <f t="shared" si="8"/>
+      <c r="P5" s="10">
+        <f>_xlfn.RANK.EQ($O5, $O$2:$O$52) +COUNTIF(O$2:O5,O5) -1</f>
         <v>30</v>
       </c>
     </row>
@@ -1504,8 +1511,8 @@
         <f t="shared" si="1"/>
         <v>-5.7149963352064452E-2</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
+      <c r="F6" s="9">
+        <f>_xlfn.RANK.EQ($E6, $E$2:$E$52) +COUNTIF(E$2:E6,E6) -1</f>
         <v>41</v>
       </c>
       <c r="G6">
@@ -1515,15 +1522,15 @@
         <v>427758.64</v>
       </c>
       <c r="I6">
+        <f t="shared" si="2"/>
+        <v>-741.35999999998603</v>
+      </c>
+      <c r="J6" s="5">
         <f t="shared" si="3"/>
-        <v>-741.35999999998603</v>
-      </c>
-      <c r="J6" s="5">
-        <f t="shared" si="4"/>
         <v>-1.7301283547257551E-3</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="5"/>
+      <c r="K6" s="10">
+        <f>_xlfn.RANK.EQ($J6, $J$2:$J$52) +COUNTIF(J$2:J6,J6) -1</f>
         <v>8</v>
       </c>
       <c r="L6">
@@ -1533,15 +1540,15 @@
         <v>445114.28999999899</v>
       </c>
       <c r="N6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-85.710000001010485</v>
       </c>
       <c r="O6" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.925202156356929E-4</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="8"/>
+      <c r="P6" s="10">
+        <f>_xlfn.RANK.EQ($O6, $O$2:$O$52) +COUNTIF(O$2:O6,O6) -1</f>
         <v>13</v>
       </c>
     </row>
@@ -1563,8 +1570,8 @@
         <f t="shared" si="1"/>
         <v>-0.11502817362571344</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
+      <c r="F7" s="9">
+        <f>_xlfn.RANK.EQ($E7, $E$2:$E$52) +COUNTIF(E$2:E7,E7) -1</f>
         <v>50</v>
       </c>
       <c r="G7">
@@ -1574,15 +1581,15 @@
         <v>3051483.41</v>
       </c>
       <c r="I7">
+        <f t="shared" si="2"/>
+        <v>-339416.58999999985</v>
+      </c>
+      <c r="J7" s="5">
         <f t="shared" si="3"/>
-        <v>-339416.58999999985</v>
-      </c>
-      <c r="J7" s="5">
-        <f t="shared" si="4"/>
         <v>-0.10009631366303927</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="5"/>
+      <c r="K7" s="10">
+        <f>_xlfn.RANK.EQ($J7, $J$2:$J$52) +COUNTIF(J$2:J7,J7) -1</f>
         <v>44</v>
       </c>
       <c r="L7">
@@ -1592,15 +1599,15 @@
         <v>2946440.08</v>
       </c>
       <c r="N7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-398759.91999999993</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-0.11920361114432618</v>
       </c>
-      <c r="P7">
-        <f t="shared" si="8"/>
+      <c r="P7" s="10">
+        <f>_xlfn.RANK.EQ($O7, $O$2:$O$52) +COUNTIF(O$2:O7,O7) -1</f>
         <v>48</v>
       </c>
     </row>
@@ -1622,8 +1629,8 @@
         <f t="shared" si="1"/>
         <v>-0.15235918433091292</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
+      <c r="F8" s="9">
+        <f>_xlfn.RANK.EQ($E8, $E$2:$E$52) +COUNTIF(E$2:E8,E8) -1</f>
         <v>51</v>
       </c>
       <c r="G8">
@@ -1633,15 +1640,15 @@
         <v>1383905.98999999</v>
       </c>
       <c r="I8">
+        <f t="shared" si="2"/>
+        <v>-206794.01000001002</v>
+      </c>
+      <c r="J8" s="5">
         <f t="shared" si="3"/>
-        <v>-206794.01000001002</v>
-      </c>
-      <c r="J8" s="5">
-        <f t="shared" si="4"/>
         <v>-0.13000189224870184</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="5"/>
+      <c r="K8" s="10">
+        <f>_xlfn.RANK.EQ($J8, $J$2:$J$52) +COUNTIF(J$2:J8,J8) -1</f>
         <v>48</v>
       </c>
       <c r="L8">
@@ -1651,15 +1658,15 @@
         <v>1337735.3199999901</v>
       </c>
       <c r="N8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-241564.68000000995</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-0.15295680364719175</v>
       </c>
-      <c r="P8">
-        <f t="shared" si="8"/>
+      <c r="P8" s="10">
+        <f>_xlfn.RANK.EQ($O8, $O$2:$O$52) +COUNTIF(O$2:O8,O8) -1</f>
         <v>50</v>
       </c>
     </row>
@@ -1681,8 +1688,8 @@
         <f t="shared" si="1"/>
         <v>-4.2417130511048909E-2</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
+      <c r="F9" s="9">
+        <f>_xlfn.RANK.EQ($E9, $E$2:$E$52) +COUNTIF(E$2:E9,E9) -1</f>
         <v>36</v>
       </c>
       <c r="G9">
@@ -1692,15 +1699,15 @@
         <v>9929059.5199999996</v>
       </c>
       <c r="I9">
+        <f t="shared" si="2"/>
+        <v>-1144640.4800000004</v>
+      </c>
+      <c r="J9" s="5">
         <f t="shared" si="3"/>
-        <v>-1144640.4800000004</v>
-      </c>
-      <c r="J9" s="5">
-        <f t="shared" si="4"/>
         <v>-0.10336567542917005</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="5"/>
+      <c r="K9" s="10">
+        <f>_xlfn.RANK.EQ($J9, $J$2:$J$52) +COUNTIF(J$2:J9,J9) -1</f>
         <v>45</v>
       </c>
       <c r="L9">
@@ -1710,15 +1717,15 @@
         <v>9993599.52999999</v>
       </c>
       <c r="N9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-796900.47000000998</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-7.3852043000788653E-2</v>
       </c>
-      <c r="P9">
-        <f t="shared" si="8"/>
+      <c r="P9" s="10">
+        <f>_xlfn.RANK.EQ($O9, $O$2:$O$52) +COUNTIF(O$2:O9,O9) -1</f>
         <v>43</v>
       </c>
     </row>
@@ -1740,8 +1747,8 @@
         <f t="shared" si="1"/>
         <v>-8.1681998646514792E-2</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
+      <c r="F10" s="9">
+        <f>_xlfn.RANK.EQ($E10, $E$2:$E$52) +COUNTIF(E$2:E10,E10) -1</f>
         <v>46</v>
       </c>
       <c r="G10">
@@ -1751,15 +1758,15 @@
         <v>467907.84000000003</v>
       </c>
       <c r="I10">
+        <f t="shared" si="2"/>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="J10" s="5">
         <f t="shared" si="3"/>
-        <v>-27292.159999999974</v>
-      </c>
-      <c r="J10" s="5">
-        <f t="shared" si="4"/>
         <v>-5.5113408723747932E-2</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="5"/>
+      <c r="K10" s="10">
+        <f>_xlfn.RANK.EQ($J10, $J$2:$J$52) +COUNTIF(J$2:J10,J10) -1</f>
         <v>35</v>
       </c>
       <c r="L10">
@@ -1769,15 +1776,15 @@
         <v>478318.92</v>
       </c>
       <c r="N10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-9181.0800000000163</v>
       </c>
       <c r="O10" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.883298461538465E-2</v>
       </c>
-      <c r="P10">
-        <f t="shared" si="8"/>
+      <c r="P10" s="10">
+        <f>_xlfn.RANK.EQ($O10, $O$2:$O$52) +COUNTIF(O$2:O10,O10) -1</f>
         <v>23</v>
       </c>
     </row>
@@ -1799,26 +1806,26 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="9">
+        <f>_xlfn.RANK.EQ($E11, $E$2:$E$52) +COUNTIF(E$2:E11,E11) -1</f>
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J11" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="5"/>
+      <c r="K11" s="10">
+        <f>_xlfn.RANK.EQ($J11, $J$2:$J$52) +COUNTIF(J$2:J11,J11) -1</f>
         <v>1</v>
       </c>
       <c r="L11">
@@ -1828,15 +1835,15 @@
         <v>63771.91</v>
       </c>
       <c r="N11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-311228.08999999997</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-0.82994157333333329</v>
       </c>
-      <c r="P11">
-        <f t="shared" si="8"/>
+      <c r="P11" s="10">
+        <f>_xlfn.RANK.EQ($O11, $O$2:$O$52) +COUNTIF(O$2:O11,O11) -1</f>
         <v>51</v>
       </c>
     </row>
@@ -1858,8 +1865,8 @@
         <f t="shared" si="1"/>
         <v>-5.0060657805601608E-2</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
+      <c r="F12" s="9">
+        <f>_xlfn.RANK.EQ($E12, $E$2:$E$52) +COUNTIF(E$2:E12,E12) -1</f>
         <v>39</v>
       </c>
       <c r="G12">
@@ -1869,15 +1876,15 @@
         <v>4205555.5999999996</v>
       </c>
       <c r="I12">
+        <f t="shared" si="2"/>
+        <v>-494844.40000000037</v>
+      </c>
+      <c r="J12" s="5">
         <f t="shared" si="3"/>
-        <v>-494844.40000000037</v>
-      </c>
-      <c r="J12" s="5">
-        <f t="shared" si="4"/>
         <v>-0.10527708280146378</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="5"/>
+      <c r="K12" s="10">
+        <f>_xlfn.RANK.EQ($J12, $J$2:$J$52) +COUNTIF(J$2:J12,J12) -1</f>
         <v>46</v>
       </c>
       <c r="L12">
@@ -1887,15 +1894,15 @@
         <v>4371713.1399999997</v>
       </c>
       <c r="N12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-306086.86000000034</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-6.5433934755654441E-2</v>
       </c>
-      <c r="P12">
-        <f t="shared" si="8"/>
+      <c r="P12" s="10">
+        <f>_xlfn.RANK.EQ($O12, $O$2:$O$52) +COUNTIF(O$2:O12,O12) -1</f>
         <v>42</v>
       </c>
     </row>
@@ -1917,8 +1924,8 @@
         <f t="shared" si="1"/>
         <v>-1.2912833886247806E-2</v>
       </c>
-      <c r="F13">
-        <f t="shared" si="2"/>
+      <c r="F13" s="9">
+        <f>_xlfn.RANK.EQ($E13, $E$2:$E$52) +COUNTIF(E$2:E13,E13) -1</f>
         <v>19</v>
       </c>
       <c r="G13">
@@ -1928,15 +1935,15 @@
         <v>5909077.9399999902</v>
       </c>
       <c r="I13">
+        <f t="shared" si="2"/>
+        <v>-314622.06000000983</v>
+      </c>
+      <c r="J13" s="5">
         <f t="shared" si="3"/>
-        <v>-314622.06000000983</v>
-      </c>
-      <c r="J13" s="5">
-        <f t="shared" si="4"/>
         <v>-5.0552253482656594E-2</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="5"/>
+      <c r="K13" s="10">
+        <f>_xlfn.RANK.EQ($J13, $J$2:$J$52) +COUNTIF(J$2:J13,J13) -1</f>
         <v>34</v>
       </c>
       <c r="L13">
@@ -1946,15 +1953,15 @@
         <v>6056976.6699999999</v>
       </c>
       <c r="N13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-150323.33000000007</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.4217184605222895E-2</v>
       </c>
-      <c r="P13">
-        <f t="shared" si="8"/>
+      <c r="P13" s="10">
+        <f>_xlfn.RANK.EQ($O13, $O$2:$O$52) +COUNTIF(O$2:O13,O13) -1</f>
         <v>25</v>
       </c>
     </row>
@@ -1976,8 +1983,8 @@
         <f t="shared" si="1"/>
         <v>-1.3637949218750009E-2</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="2"/>
+      <c r="F14" s="9">
+        <f>_xlfn.RANK.EQ($E14, $E$2:$E$52) +COUNTIF(E$2:E14,E14) -1</f>
         <v>22</v>
       </c>
       <c r="G14">
@@ -1987,15 +1994,15 @@
         <v>524402.98</v>
       </c>
       <c r="I14">
+        <f t="shared" si="2"/>
+        <v>-6097.0200000000186</v>
+      </c>
+      <c r="J14" s="5">
         <f t="shared" si="3"/>
-        <v>-6097.0200000000186</v>
-      </c>
-      <c r="J14" s="5">
-        <f t="shared" si="4"/>
         <v>-1.1492968897266765E-2</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="5"/>
+      <c r="K14" s="10">
+        <f>_xlfn.RANK.EQ($J14, $J$2:$J$52) +COUNTIF(J$2:J14,J14) -1</f>
         <v>12</v>
       </c>
       <c r="L14">
@@ -2005,15 +2012,15 @@
         <v>504989.88</v>
       </c>
       <c r="N14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-21210.119999999995</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-4.0308095781071827E-2</v>
       </c>
-      <c r="P14">
-        <f t="shared" si="8"/>
+      <c r="P14" s="10">
+        <f>_xlfn.RANK.EQ($O14, $O$2:$O$52) +COUNTIF(O$2:O14,O14) -1</f>
         <v>33</v>
       </c>
     </row>
@@ -2035,8 +2042,8 @@
         <f t="shared" si="1"/>
         <v>3.1837408866824991E-3</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="2"/>
+      <c r="F15" s="9">
+        <f>_xlfn.RANK.EQ($E15, $E$2:$E$52) +COUNTIF(E$2:E15,E15) -1</f>
         <v>1</v>
       </c>
       <c r="G15">
@@ -2046,15 +2053,15 @@
         <v>175966389.24999899</v>
       </c>
       <c r="I15">
+        <f t="shared" si="2"/>
+        <v>-8201410.7500010133</v>
+      </c>
+      <c r="J15" s="5">
         <f t="shared" si="3"/>
-        <v>-8201410.7500010133</v>
-      </c>
-      <c r="J15" s="5">
-        <f t="shared" si="4"/>
         <v>-4.4532273014072019E-2</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="5"/>
+      <c r="K15" s="10">
+        <f>_xlfn.RANK.EQ($J15, $J$2:$J$52) +COUNTIF(J$2:J15,J15) -1</f>
         <v>28</v>
       </c>
       <c r="L15">
@@ -2064,15 +2071,15 @@
         <v>184450910.84999901</v>
       </c>
       <c r="N15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-4502589.1500009894</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.3829085727446114E-2</v>
       </c>
-      <c r="P15">
-        <f t="shared" si="8"/>
+      <c r="P15" s="10">
+        <f>_xlfn.RANK.EQ($O15, $O$2:$O$52) +COUNTIF(O$2:O15,O15) -1</f>
         <v>24</v>
       </c>
     </row>
@@ -2094,8 +2101,8 @@
         <f t="shared" si="1"/>
         <v>-1.1850188616360429E-2</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="2"/>
+      <c r="F16" s="9">
+        <f>_xlfn.RANK.EQ($E16, $E$2:$E$52) +COUNTIF(E$2:E16,E16) -1</f>
         <v>15</v>
       </c>
       <c r="G16">
@@ -2105,15 +2112,15 @@
         <v>7350464.0800000001</v>
       </c>
       <c r="I16">
+        <f t="shared" si="2"/>
+        <v>-2035.9199999999255</v>
+      </c>
+      <c r="J16" s="5">
         <f t="shared" si="3"/>
-        <v>-2035.9199999999255</v>
-      </c>
-      <c r="J16" s="5">
-        <f t="shared" si="4"/>
         <v>-2.769017341040361E-4</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="5"/>
+      <c r="K16" s="10">
+        <f>_xlfn.RANK.EQ($J16, $J$2:$J$52) +COUNTIF(J$2:J16,J16) -1</f>
         <v>6</v>
       </c>
       <c r="L16">
@@ -2123,15 +2130,15 @@
         <v>7397093</v>
       </c>
       <c r="N16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-107</v>
       </c>
       <c r="O16" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.4464932677229222E-5</v>
       </c>
-      <c r="P16">
-        <f t="shared" si="8"/>
+      <c r="P16" s="10">
+        <f>_xlfn.RANK.EQ($O16, $O$2:$O$52) +COUNTIF(O$2:O16,O16) -1</f>
         <v>9</v>
       </c>
     </row>
@@ -2153,8 +2160,8 @@
         <f t="shared" si="1"/>
         <v>-2.8351094826658003E-2</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="2"/>
+      <c r="F17" s="9">
+        <f>_xlfn.RANK.EQ($E17, $E$2:$E$52) +COUNTIF(E$2:E17,E17) -1</f>
         <v>31</v>
       </c>
       <c r="G17">
@@ -2164,15 +2171,15 @@
         <v>14645233.51</v>
       </c>
       <c r="I17">
+        <f t="shared" si="2"/>
+        <v>-664466.49000000022</v>
+      </c>
+      <c r="J17" s="5">
         <f t="shared" si="3"/>
-        <v>-664466.49000000022</v>
-      </c>
-      <c r="J17" s="5">
-        <f t="shared" si="4"/>
         <v>-4.3401666263871937E-2</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="5"/>
+      <c r="K17" s="10">
+        <f>_xlfn.RANK.EQ($J17, $J$2:$J$52) +COUNTIF(J$2:J17,J17) -1</f>
         <v>27</v>
       </c>
       <c r="L17">
@@ -2182,15 +2189,15 @@
         <v>14346057.039999999</v>
       </c>
       <c r="N17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-965742.96000000089</v>
       </c>
       <c r="O17" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-6.3071811282801551E-2</v>
       </c>
-      <c r="P17">
-        <f t="shared" si="8"/>
+      <c r="P17" s="10">
+        <f>_xlfn.RANK.EQ($O17, $O$2:$O$52) +COUNTIF(O$2:O17,O17) -1</f>
         <v>41</v>
       </c>
     </row>
@@ -2212,8 +2219,8 @@
         <f t="shared" si="1"/>
         <v>-5.4037002206391245E-2</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="2"/>
+      <c r="F18" s="9">
+        <f>_xlfn.RANK.EQ($E18, $E$2:$E$52) +COUNTIF(E$2:E18,E18) -1</f>
         <v>40</v>
       </c>
       <c r="G18">
@@ -2223,15 +2230,15 @@
         <v>2671745.94</v>
       </c>
       <c r="I18">
+        <f t="shared" si="2"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="J18" s="5">
         <f t="shared" si="3"/>
-        <v>-189254.06000000006</v>
-      </c>
-      <c r="J18" s="5">
-        <f t="shared" si="4"/>
         <v>-6.6149619014330668E-2</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="5"/>
+      <c r="K18" s="10">
+        <f>_xlfn.RANK.EQ($J18, $J$2:$J$52) +COUNTIF(J$2:J18,J18) -1</f>
         <v>37</v>
       </c>
       <c r="L18">
@@ -2241,15 +2248,15 @@
         <v>2535637.09</v>
       </c>
       <c r="N18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-374962.91000000015</v>
       </c>
       <c r="O18" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-0.12882667147667154</v>
       </c>
-      <c r="P18">
-        <f t="shared" si="8"/>
+      <c r="P18" s="10">
+        <f>_xlfn.RANK.EQ($O18, $O$2:$O$52) +COUNTIF(O$2:O18,O18) -1</f>
         <v>49</v>
       </c>
     </row>
@@ -2271,8 +2278,8 @@
         <f t="shared" si="1"/>
         <v>-4.258504294298146E-2</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="2"/>
+      <c r="F19" s="9">
+        <f>_xlfn.RANK.EQ($E19, $E$2:$E$52) +COUNTIF(E$2:E19,E19) -1</f>
         <v>37</v>
       </c>
       <c r="G19">
@@ -2282,15 +2289,15 @@
         <v>8991707.2399999909</v>
       </c>
       <c r="I19">
+        <f t="shared" si="2"/>
+        <v>-721592.76000000909</v>
+      </c>
+      <c r="J19" s="5">
         <f t="shared" si="3"/>
-        <v>-721592.76000000909</v>
-      </c>
-      <c r="J19" s="5">
-        <f t="shared" si="4"/>
         <v>-7.4289145810384635E-2</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="5"/>
+      <c r="K19" s="10">
+        <f>_xlfn.RANK.EQ($J19, $J$2:$J$52) +COUNTIF(J$2:J19,J19) -1</f>
         <v>40</v>
       </c>
       <c r="L19">
@@ -2300,15 +2307,15 @@
         <v>8766655.9100000001</v>
       </c>
       <c r="N19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-576344.08999999985</v>
       </c>
       <c r="O19" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-6.1687262121374278E-2</v>
       </c>
-      <c r="P19">
-        <f t="shared" si="8"/>
+      <c r="P19" s="10">
+        <f>_xlfn.RANK.EQ($O19, $O$2:$O$52) +COUNTIF(O$2:O19,O19) -1</f>
         <v>40</v>
       </c>
     </row>
@@ -2330,8 +2337,8 @@
         <f t="shared" si="1"/>
         <v>-1.2379538203300809E-5</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="2"/>
+      <c r="F20" s="9">
+        <f>_xlfn.RANK.EQ($E20, $E$2:$E$52) +COUNTIF(E$2:E20,E20) -1</f>
         <v>6</v>
       </c>
       <c r="G20">
@@ -2341,15 +2348,15 @@
         <v>131839624.37</v>
       </c>
       <c r="I20">
+        <f t="shared" si="2"/>
+        <v>-9775.6299999952316</v>
+      </c>
+      <c r="J20" s="5">
         <f t="shared" si="3"/>
-        <v>-9775.6299999952316</v>
-      </c>
-      <c r="J20" s="5">
-        <f t="shared" si="4"/>
         <v>-7.4142392760188761E-5</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="5"/>
+      <c r="K20" s="10">
+        <f>_xlfn.RANK.EQ($J20, $J$2:$J$52) +COUNTIF(J$2:J20,J20) -1</f>
         <v>5</v>
       </c>
       <c r="L20">
@@ -2359,15 +2366,15 @@
         <v>130621283.53999899</v>
       </c>
       <c r="N20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-116.46000100672245</v>
       </c>
       <c r="O20" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-8.9158438821450736E-7</v>
       </c>
-      <c r="P20">
-        <f t="shared" si="8"/>
+      <c r="P20" s="10">
+        <f>_xlfn.RANK.EQ($O20, $O$2:$O$52) +COUNTIF(O$2:O20,O20) -1</f>
         <v>6</v>
       </c>
     </row>
@@ -2389,8 +2396,8 @@
         <f t="shared" si="1"/>
         <v>-7.9052463618023094E-2</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="2"/>
+      <c r="F21" s="9">
+        <f>_xlfn.RANK.EQ($E21, $E$2:$E$52) +COUNTIF(E$2:E21,E21) -1</f>
         <v>43</v>
       </c>
       <c r="G21">
@@ -2400,15 +2407,15 @@
         <v>22655993.629999999</v>
       </c>
       <c r="I21">
+        <f t="shared" si="2"/>
+        <v>-1841406.370000001</v>
+      </c>
+      <c r="J21" s="5">
         <f t="shared" si="3"/>
-        <v>-1841406.370000001</v>
-      </c>
-      <c r="J21" s="5">
-        <f t="shared" si="4"/>
         <v>-7.5167420624229556E-2</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="5"/>
+      <c r="K21" s="10">
+        <f>_xlfn.RANK.EQ($J21, $J$2:$J$52) +COUNTIF(J$2:J21,J21) -1</f>
         <v>41</v>
       </c>
       <c r="L21">
@@ -2418,15 +2425,15 @@
         <v>23434073.089999899</v>
       </c>
       <c r="N21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-888926.91000010073</v>
       </c>
       <c r="O21" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-3.6546762734864152E-2</v>
       </c>
-      <c r="P21">
-        <f t="shared" si="8"/>
+      <c r="P21" s="10">
+        <f>_xlfn.RANK.EQ($O21, $O$2:$O$52) +COUNTIF(O$2:O21,O21) -1</f>
         <v>31</v>
       </c>
     </row>
@@ -2448,8 +2455,8 @@
         <f t="shared" si="1"/>
         <v>-1.3285502334437123E-2</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="2"/>
+      <c r="F22" s="9">
+        <f>_xlfn.RANK.EQ($E22, $E$2:$E$52) +COUNTIF(E$2:E22,E22) -1</f>
         <v>20</v>
       </c>
       <c r="G22">
@@ -2459,15 +2466,15 @@
         <v>11791977.9699999</v>
       </c>
       <c r="I22">
+        <f t="shared" si="2"/>
+        <v>-188722.03000009991</v>
+      </c>
+      <c r="J22" s="5">
         <f t="shared" si="3"/>
-        <v>-188722.03000009991</v>
-      </c>
-      <c r="J22" s="5">
-        <f t="shared" si="4"/>
         <v>-1.5752170574348738E-2</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="5"/>
+      <c r="K22" s="10">
+        <f>_xlfn.RANK.EQ($J22, $J$2:$J$52) +COUNTIF(J$2:J22,J22) -1</f>
         <v>14</v>
       </c>
       <c r="L22">
@@ -2477,15 +2484,15 @@
         <v>11934454.77</v>
       </c>
       <c r="N22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-745.23000000044703</v>
       </c>
       <c r="O22" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-6.2439674240938325E-5</v>
       </c>
-      <c r="P22">
-        <f t="shared" si="8"/>
+      <c r="P22" s="10">
+        <f>_xlfn.RANK.EQ($O22, $O$2:$O$52) +COUNTIF(O$2:O22,O22) -1</f>
         <v>10</v>
       </c>
     </row>
@@ -2507,8 +2514,8 @@
         <f t="shared" si="1"/>
         <v>-3.9590110100806722E-2</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="2"/>
+      <c r="F23" s="9">
+        <f>_xlfn.RANK.EQ($E23, $E$2:$E$52) +COUNTIF(E$2:E23,E23) -1</f>
         <v>34</v>
       </c>
       <c r="G23">
@@ -2518,15 +2525,15 @@
         <v>21722126.219999898</v>
       </c>
       <c r="I23">
+        <f t="shared" si="2"/>
+        <v>-961673.78000010177</v>
+      </c>
+      <c r="J23" s="5">
         <f t="shared" si="3"/>
-        <v>-961673.78000010177</v>
-      </c>
-      <c r="J23" s="5">
-        <f t="shared" si="4"/>
         <v>-4.2394738976719144E-2</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="5"/>
+      <c r="K23" s="10">
+        <f>_xlfn.RANK.EQ($J23, $J$2:$J$52) +COUNTIF(J$2:J23,J23) -1</f>
         <v>26</v>
       </c>
       <c r="L23">
@@ -2536,15 +2543,15 @@
         <v>22619057.440000001</v>
       </c>
       <c r="N23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-601242.55999999866</v>
       </c>
       <c r="O23" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.5892971236375011E-2</v>
       </c>
-      <c r="P23">
-        <f t="shared" si="8"/>
+      <c r="P23" s="10">
+        <f>_xlfn.RANK.EQ($O23, $O$2:$O$52) +COUNTIF(O$2:O23,O23) -1</f>
         <v>26</v>
       </c>
     </row>
@@ -2566,8 +2573,8 @@
         <f t="shared" si="1"/>
         <v>-1.3334943305713101E-2</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="2"/>
+      <c r="F24" s="9">
+        <f>_xlfn.RANK.EQ($E24, $E$2:$E$52) +COUNTIF(E$2:E24,E24) -1</f>
         <v>21</v>
       </c>
       <c r="G24">
@@ -2577,15 +2584,15 @@
         <v>1067214.42</v>
       </c>
       <c r="I24">
+        <f t="shared" si="2"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="J24" s="5">
         <f t="shared" si="3"/>
-        <v>-45485.580000000075</v>
-      </c>
-      <c r="J24" s="5">
-        <f t="shared" si="4"/>
         <v>-4.087856565111897E-2</v>
       </c>
-      <c r="K24">
-        <f t="shared" si="5"/>
+      <c r="K24" s="10">
+        <f>_xlfn.RANK.EQ($J24, $J$2:$J$52) +COUNTIF(J$2:J24,J24) -1</f>
         <v>24</v>
       </c>
       <c r="L24">
@@ -2595,15 +2602,15 @@
         <v>1112527.1200000001</v>
       </c>
       <c r="N24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-72.879999999888241</v>
       </c>
       <c r="O24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-6.5504224339284781E-5</v>
       </c>
-      <c r="P24">
-        <f t="shared" si="8"/>
+      <c r="P24" s="10">
+        <f>_xlfn.RANK.EQ($O24, $O$2:$O$52) +COUNTIF(O$2:O24,O24) -1</f>
         <v>11</v>
       </c>
     </row>
@@ -2625,8 +2632,8 @@
         <f t="shared" si="1"/>
         <v>-1.0226130964676661E-2</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="2"/>
+      <c r="F25" s="9">
+        <f>_xlfn.RANK.EQ($E25, $E$2:$E$52) +COUNTIF(E$2:E25,E25) -1</f>
         <v>14</v>
       </c>
       <c r="G25">
@@ -2636,15 +2643,15 @@
         <v>497194.20999999897</v>
       </c>
       <c r="I25">
+        <f t="shared" si="2"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="J25" s="5">
         <f t="shared" si="3"/>
-        <v>-8005.7900000010268</v>
-      </c>
-      <c r="J25" s="5">
-        <f t="shared" si="4"/>
         <v>-1.5846773555029746E-2</v>
       </c>
-      <c r="K25">
-        <f t="shared" si="5"/>
+      <c r="K25" s="10">
+        <f>_xlfn.RANK.EQ($J25, $J$2:$J$52) +COUNTIF(J$2:J25,J25) -1</f>
         <v>15</v>
       </c>
       <c r="L25">
@@ -2654,15 +2661,15 @@
         <v>494775.1</v>
       </c>
       <c r="N25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-1724.9000000000233</v>
       </c>
       <c r="O25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-3.4741188318228064E-3</v>
       </c>
-      <c r="P25">
-        <f t="shared" si="8"/>
+      <c r="P25" s="10">
+        <f>_xlfn.RANK.EQ($O25, $O$2:$O$52) +COUNTIF(O$2:O25,O25) -1</f>
         <v>17</v>
       </c>
     </row>
@@ -2684,8 +2691,8 @@
         <f t="shared" si="1"/>
         <v>-8.5306091660634673E-2</v>
       </c>
-      <c r="F26">
-        <f t="shared" si="2"/>
+      <c r="F26" s="9">
+        <f>_xlfn.RANK.EQ($E26, $E$2:$E$52) +COUNTIF(E$2:E26,E26) -1</f>
         <v>47</v>
       </c>
       <c r="G26">
@@ -2695,15 +2702,15 @@
         <v>5122329.02999999</v>
       </c>
       <c r="I26">
+        <f t="shared" si="2"/>
+        <v>-319870.97000000998</v>
+      </c>
+      <c r="J26" s="5">
         <f t="shared" si="3"/>
-        <v>-319870.97000000998</v>
-      </c>
-      <c r="J26" s="5">
-        <f t="shared" si="4"/>
         <v>-5.8776040939327839E-2</v>
       </c>
-      <c r="K26">
-        <f t="shared" si="5"/>
+      <c r="K26" s="10">
+        <f>_xlfn.RANK.EQ($J26, $J$2:$J$52) +COUNTIF(J$2:J26,J26) -1</f>
         <v>36</v>
       </c>
       <c r="L26">
@@ -2713,15 +2720,15 @@
         <v>5117235.21</v>
       </c>
       <c r="N26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-313464.79000000004</v>
       </c>
       <c r="O26" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-5.7720881286022069E-2</v>
       </c>
-      <c r="P26">
-        <f t="shared" si="8"/>
+      <c r="P26" s="10">
+        <f>_xlfn.RANK.EQ($O26, $O$2:$O$52) +COUNTIF(O$2:O26,O26) -1</f>
         <v>39</v>
       </c>
     </row>
@@ -2743,44 +2750,44 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="9">
+        <f>_xlfn.RANK.EQ($E27, $E$2:$E$52) +COUNTIF(E$2:E27,E27) -1</f>
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="10">
+        <f>_xlfn.RANK.EQ($J27, $J$2:$J$52) +COUNTIF(J$2:J27,J27) -1</f>
         <v>2</v>
       </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="5">
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K27">
+      <c r="O27" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="10">
+        <f>_xlfn.RANK.EQ($O27, $O$2:$O$52) +COUNTIF(O$2:O27,O27) -1</f>
         <v>1</v>
       </c>
     </row>
@@ -2802,8 +2809,8 @@
         <f t="shared" si="1"/>
         <v>-9.5782760864849215E-2</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="2"/>
+      <c r="F28" s="9">
+        <f>_xlfn.RANK.EQ($E28, $E$2:$E$52) +COUNTIF(E$2:E28,E28) -1</f>
         <v>49</v>
       </c>
       <c r="G28">
@@ -2813,15 +2820,15 @@
         <v>1281335.23</v>
       </c>
       <c r="I28">
+        <f t="shared" si="2"/>
+        <v>-264364.77</v>
+      </c>
+      <c r="J28" s="5">
         <f t="shared" si="3"/>
-        <v>-264364.77</v>
-      </c>
-      <c r="J28" s="5">
-        <f t="shared" si="4"/>
         <v>-0.17103239309050916</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="5"/>
+      <c r="K28" s="10">
+        <f>_xlfn.RANK.EQ($J28, $J$2:$J$52) +COUNTIF(J$2:J28,J28) -1</f>
         <v>50</v>
       </c>
       <c r="L28">
@@ -2831,15 +2838,15 @@
         <v>1393285.06</v>
       </c>
       <c r="N28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-132614.93999999994</v>
       </c>
       <c r="O28" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-8.6909325643882263E-2</v>
       </c>
-      <c r="P28">
-        <f t="shared" si="8"/>
+      <c r="P28" s="10">
+        <f>_xlfn.RANK.EQ($O28, $O$2:$O$52) +COUNTIF(O$2:O28,O28) -1</f>
         <v>45</v>
       </c>
     </row>
@@ -2861,8 +2868,8 @@
         <f t="shared" si="1"/>
         <v>-1.4800253727847622E-2</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="2"/>
+      <c r="F29" s="9">
+        <f>_xlfn.RANK.EQ($E29, $E$2:$E$52) +COUNTIF(E$2:E29,E29) -1</f>
         <v>24</v>
       </c>
       <c r="G29">
@@ -2872,15 +2879,15 @@
         <v>2665264.4399999902</v>
       </c>
       <c r="I29">
+        <f t="shared" si="2"/>
+        <v>-114235.56000000983</v>
+      </c>
+      <c r="J29" s="5">
         <f t="shared" si="3"/>
-        <v>-114235.56000000983</v>
-      </c>
-      <c r="J29" s="5">
-        <f t="shared" si="4"/>
         <v>-4.1099320021590155E-2</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="5"/>
+      <c r="K29" s="10">
+        <f>_xlfn.RANK.EQ($J29, $J$2:$J$52) +COUNTIF(J$2:J29,J29) -1</f>
         <v>25</v>
       </c>
       <c r="L29">
@@ -2890,15 +2897,15 @@
         <v>2889864.67</v>
       </c>
       <c r="N29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-35.330000000074506</v>
       </c>
       <c r="O29" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.2225336516860273E-5</v>
       </c>
-      <c r="P29">
-        <f t="shared" si="8"/>
+      <c r="P29" s="10">
+        <f>_xlfn.RANK.EQ($O29, $O$2:$O$52) +COUNTIF(O$2:O29,O29) -1</f>
         <v>8</v>
       </c>
     </row>
@@ -2920,8 +2927,8 @@
         <f t="shared" si="1"/>
         <v>-8.3831374359143746E-3</v>
       </c>
-      <c r="F30">
-        <f t="shared" si="2"/>
+      <c r="F30" s="9">
+        <f>_xlfn.RANK.EQ($E30, $E$2:$E$52) +COUNTIF(E$2:E30,E30) -1</f>
         <v>12</v>
       </c>
       <c r="G30">
@@ -2931,15 +2938,15 @@
         <v>12685514.279999901</v>
       </c>
       <c r="I30">
+        <f t="shared" si="2"/>
+        <v>-50385.720000099391</v>
+      </c>
+      <c r="J30" s="5">
         <f t="shared" si="3"/>
-        <v>-50385.720000099391</v>
-      </c>
-      <c r="J30" s="5">
-        <f t="shared" si="4"/>
         <v>-3.9561962641116366E-3</v>
       </c>
-      <c r="K30">
-        <f t="shared" si="5"/>
+      <c r="K30" s="10">
+        <f>_xlfn.RANK.EQ($J30, $J$2:$J$52) +COUNTIF(J$2:J30,J30) -1</f>
         <v>10</v>
       </c>
       <c r="L30">
@@ -2949,15 +2956,15 @@
         <v>12826009.609999999</v>
       </c>
       <c r="N30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-35290.390000000596</v>
       </c>
       <c r="O30" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.7439209100169185E-3</v>
       </c>
-      <c r="P30">
-        <f t="shared" si="8"/>
+      <c r="P30" s="10">
+        <f>_xlfn.RANK.EQ($O30, $O$2:$O$52) +COUNTIF(O$2:O30,O30) -1</f>
         <v>16</v>
       </c>
     </row>
@@ -2979,8 +2986,8 @@
         <f t="shared" si="1"/>
         <v>-1.4030533529678329E-2</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="2"/>
+      <c r="F31" s="9">
+        <f>_xlfn.RANK.EQ($E31, $E$2:$E$52) +COUNTIF(E$2:E31,E31) -1</f>
         <v>23</v>
       </c>
       <c r="G31">
@@ -2990,15 +2997,15 @@
         <v>1762676.85</v>
       </c>
       <c r="I31">
+        <f t="shared" si="2"/>
+        <v>-60623.149999999907</v>
+      </c>
+      <c r="J31" s="5">
         <f t="shared" si="3"/>
-        <v>-60623.149999999907</v>
-      </c>
-      <c r="J31" s="5">
-        <f t="shared" si="4"/>
         <v>-3.3249136181648611E-2</v>
       </c>
-      <c r="K31">
-        <f t="shared" si="5"/>
+      <c r="K31" s="10">
+        <f>_xlfn.RANK.EQ($J31, $J$2:$J$52) +COUNTIF(J$2:J31,J31) -1</f>
         <v>20</v>
       </c>
       <c r="L31">
@@ -3008,15 +3015,15 @@
         <v>1801391.34</v>
       </c>
       <c r="N31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-69308.659999999916</v>
       </c>
       <c r="O31" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-3.7049585716576634E-2</v>
       </c>
-      <c r="P31">
-        <f t="shared" si="8"/>
+      <c r="P31" s="10">
+        <f>_xlfn.RANK.EQ($O31, $O$2:$O$52) +COUNTIF(O$2:O31,O31) -1</f>
         <v>32</v>
       </c>
     </row>
@@ -3038,8 +3045,8 @@
         <f t="shared" si="1"/>
         <v>-1.2294942827617691E-2</v>
       </c>
-      <c r="F32">
-        <f t="shared" si="2"/>
+      <c r="F32" s="9">
+        <f>_xlfn.RANK.EQ($E32, $E$2:$E$52) +COUNTIF(E$2:E32,E32) -1</f>
         <v>16</v>
       </c>
       <c r="G32">
@@ -3049,15 +3056,15 @@
         <v>6084985.4699999997</v>
       </c>
       <c r="I32">
+        <f t="shared" si="2"/>
+        <v>-110514.53000000026</v>
+      </c>
+      <c r="J32" s="5">
         <f t="shared" si="3"/>
-        <v>-110514.53000000026</v>
-      </c>
-      <c r="J32" s="5">
-        <f t="shared" si="4"/>
         <v>-1.7837871035428981E-2</v>
       </c>
-      <c r="K32">
-        <f t="shared" si="5"/>
+      <c r="K32" s="10">
+        <f>_xlfn.RANK.EQ($J32, $J$2:$J$52) +COUNTIF(J$2:J32,J32) -1</f>
         <v>17</v>
       </c>
       <c r="L32">
@@ -3067,15 +3074,15 @@
         <v>5987572.0199999996</v>
       </c>
       <c r="N32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-169827.98000000045</v>
       </c>
       <c r="O32" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.7581118653977402E-2</v>
       </c>
-      <c r="P32">
-        <f t="shared" si="8"/>
+      <c r="P32" s="10">
+        <f>_xlfn.RANK.EQ($O32, $O$2:$O$52) +COUNTIF(O$2:O32,O32) -1</f>
         <v>29</v>
       </c>
     </row>
@@ -3097,8 +3104,8 @@
         <f t="shared" si="1"/>
         <v>-7.9969930789269058E-3</v>
       </c>
-      <c r="F33">
-        <f t="shared" si="2"/>
+      <c r="F33" s="9">
+        <f>_xlfn.RANK.EQ($E33, $E$2:$E$52) +COUNTIF(E$2:E33,E33) -1</f>
         <v>11</v>
       </c>
       <c r="G33">
@@ -3108,15 +3115,15 @@
         <v>977068513.48000002</v>
       </c>
       <c r="I33">
+        <f t="shared" si="2"/>
+        <v>-2602486.5199999809</v>
+      </c>
+      <c r="J33" s="5">
         <f t="shared" si="3"/>
-        <v>-2602486.5199999809</v>
-      </c>
-      <c r="J33" s="5">
-        <f t="shared" si="4"/>
         <v>-2.6564903115433454E-3</v>
       </c>
-      <c r="K33">
-        <f t="shared" si="5"/>
+      <c r="K33" s="10">
+        <f>_xlfn.RANK.EQ($J33, $J$2:$J$52) +COUNTIF(J$2:J33,J33) -1</f>
         <v>9</v>
       </c>
       <c r="L33">
@@ -3126,15 +3133,15 @@
         <v>984116289.40999901</v>
       </c>
       <c r="N33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-5456610.5900000334</v>
       </c>
       <c r="O33" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-5.5141067323084929E-3</v>
       </c>
-      <c r="P33">
-        <f t="shared" si="8"/>
+      <c r="P33" s="10">
+        <f>_xlfn.RANK.EQ($O33, $O$2:$O$52) +COUNTIF(O$2:O33,O33) -1</f>
         <v>18</v>
       </c>
     </row>
@@ -3156,8 +3163,8 @@
         <f t="shared" si="1"/>
         <v>-1.8939149738619768E-2</v>
       </c>
-      <c r="F34">
-        <f t="shared" si="2"/>
+      <c r="F34" s="9">
+        <f>_xlfn.RANK.EQ($E34, $E$2:$E$52) +COUNTIF(E$2:E34,E34) -1</f>
         <v>26</v>
       </c>
       <c r="G34">
@@ -3167,15 +3174,15 @@
         <v>4137588.7699999898</v>
       </c>
       <c r="I34">
+        <f t="shared" si="2"/>
+        <v>-213011.23000001023</v>
+      </c>
+      <c r="J34" s="5">
         <f t="shared" si="3"/>
-        <v>-213011.23000001023</v>
-      </c>
-      <c r="J34" s="5">
-        <f t="shared" si="4"/>
         <v>-4.8961345561534093E-2</v>
       </c>
-      <c r="K34">
-        <f t="shared" si="5"/>
+      <c r="K34" s="10">
+        <f>_xlfn.RANK.EQ($J34, $J$2:$J$52) +COUNTIF(J$2:J34,J34) -1</f>
         <v>31</v>
       </c>
       <c r="L34">
@@ -3185,15 +3192,15 @@
         <v>4229801.51</v>
       </c>
       <c r="N34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-115798.49000000022</v>
       </c>
       <c r="O34" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.6647296115611244E-2</v>
       </c>
-      <c r="P34">
-        <f t="shared" si="8"/>
+      <c r="P34" s="10">
+        <f>_xlfn.RANK.EQ($O34, $O$2:$O$52) +COUNTIF(O$2:O34,O34) -1</f>
         <v>28</v>
       </c>
     </row>
@@ -3215,45 +3222,45 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="9">
+        <f>_xlfn.RANK.EQ($E35, $E$2:$E$52) +COUNTIF(E$2:E35,E35) -1</f>
+        <v>4</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="10">
+        <f>_xlfn.RANK.EQ($J35, $J$2:$J$52) +COUNTIF(J$2:J35,J35) -1</f>
+        <v>3</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="10">
+        <f>_xlfn.RANK.EQ($O35, $O$2:$O$52) +COUNTIF(O$2:O35,O35) -1</f>
         <v>2</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O35" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="8"/>
-        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -3274,8 +3281,8 @@
         <f t="shared" si="1"/>
         <v>-7.8647857679780775E-2</v>
       </c>
-      <c r="F36">
-        <f t="shared" si="2"/>
+      <c r="F36" s="9">
+        <f>_xlfn.RANK.EQ($E36, $E$2:$E$52) +COUNTIF(E$2:E36,E36) -1</f>
         <v>42</v>
       </c>
       <c r="G36">
@@ -3285,15 +3292,15 @@
         <v>740966.94999999902</v>
       </c>
       <c r="I36">
+        <f t="shared" si="2"/>
+        <v>-157733.05000000098</v>
+      </c>
+      <c r="J36" s="5">
         <f t="shared" si="3"/>
-        <v>-157733.05000000098</v>
-      </c>
-      <c r="J36" s="5">
-        <f t="shared" si="4"/>
         <v>-0.17551246244575608</v>
       </c>
-      <c r="K36">
-        <f t="shared" si="5"/>
+      <c r="K36" s="10">
+        <f>_xlfn.RANK.EQ($J36, $J$2:$J$52) +COUNTIF(J$2:J36,J36) -1</f>
         <v>51</v>
       </c>
       <c r="L36">
@@ -3303,15 +3310,15 @@
         <v>777215.28999999899</v>
       </c>
       <c r="N36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-101084.71000000101</v>
       </c>
       <c r="O36" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-0.11509132414892521</v>
       </c>
-      <c r="P36">
-        <f t="shared" si="8"/>
+      <c r="P36" s="10">
+        <f>_xlfn.RANK.EQ($O36, $O$2:$O$52) +COUNTIF(O$2:O36,O36) -1</f>
         <v>47</v>
       </c>
     </row>
@@ -3333,8 +3340,8 @@
         <f t="shared" si="1"/>
         <v>-3.9444515758219188E-2</v>
       </c>
-      <c r="F37">
-        <f t="shared" si="2"/>
+      <c r="F37" s="9">
+        <f>_xlfn.RANK.EQ($E37, $E$2:$E$52) +COUNTIF(E$2:E37,E37) -1</f>
         <v>33</v>
       </c>
       <c r="G37">
@@ -3344,15 +3351,15 @@
         <v>2118943.21</v>
       </c>
       <c r="I37">
+        <f t="shared" si="2"/>
+        <v>-110256.79000000004</v>
+      </c>
+      <c r="J37" s="5">
         <f t="shared" si="3"/>
-        <v>-110256.79000000004</v>
-      </c>
-      <c r="J37" s="5">
-        <f t="shared" si="4"/>
         <v>-4.9460250314014013E-2</v>
       </c>
-      <c r="K37">
-        <f t="shared" si="5"/>
+      <c r="K37" s="10">
+        <f>_xlfn.RANK.EQ($J37, $J$2:$J$52) +COUNTIF(J$2:J37,J37) -1</f>
         <v>32</v>
       </c>
       <c r="L37">
@@ -3362,15 +3369,15 @@
         <v>2108718.34</v>
       </c>
       <c r="N37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-188181.66000000015</v>
       </c>
       <c r="O37" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-8.1928538464887526E-2</v>
       </c>
-      <c r="P37">
-        <f t="shared" si="8"/>
+      <c r="P37" s="10">
+        <f>_xlfn.RANK.EQ($O37, $O$2:$O$52) +COUNTIF(O$2:O37,O37) -1</f>
         <v>44</v>
       </c>
     </row>
@@ -3392,8 +3399,8 @@
         <f t="shared" si="1"/>
         <v>-1.9443680579913542E-2</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="2"/>
+      <c r="F38" s="9">
+        <f>_xlfn.RANK.EQ($E38, $E$2:$E$52) +COUNTIF(E$2:E38,E38) -1</f>
         <v>27</v>
       </c>
       <c r="G38">
@@ -3403,15 +3410,15 @@
         <v>753451.96</v>
       </c>
       <c r="I38">
+        <f t="shared" si="2"/>
+        <v>-39348.040000000037</v>
+      </c>
+      <c r="J38" s="5">
         <f t="shared" si="3"/>
-        <v>-39348.040000000037</v>
-      </c>
-      <c r="J38" s="5">
-        <f t="shared" si="4"/>
         <v>-4.9631735620585316E-2</v>
       </c>
-      <c r="K38">
-        <f t="shared" si="5"/>
+      <c r="K38" s="10">
+        <f>_xlfn.RANK.EQ($J38, $J$2:$J$52) +COUNTIF(J$2:J38,J38) -1</f>
         <v>33</v>
       </c>
       <c r="L38">
@@ -3421,15 +3428,15 @@
         <v>777663.26</v>
       </c>
       <c r="N38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-136.73999999999069</v>
       </c>
       <c r="O38" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.7580354847003174E-4</v>
       </c>
-      <c r="P38">
-        <f t="shared" si="8"/>
+      <c r="P38" s="10">
+        <f>_xlfn.RANK.EQ($O38, $O$2:$O$52) +COUNTIF(O$2:O38,O38) -1</f>
         <v>12</v>
       </c>
     </row>
@@ -3451,8 +3458,8 @@
         <f t="shared" si="1"/>
         <v>-8.008952370177623E-2</v>
       </c>
-      <c r="F39">
-        <f t="shared" si="2"/>
+      <c r="F39" s="9">
+        <f>_xlfn.RANK.EQ($E39, $E$2:$E$52) +COUNTIF(E$2:E39,E39) -1</f>
         <v>44</v>
       </c>
       <c r="G39">
@@ -3462,15 +3469,15 @@
         <v>1114242.27999999</v>
       </c>
       <c r="I39">
+        <f t="shared" si="2"/>
+        <v>-180157.72000000998</v>
+      </c>
+      <c r="J39" s="5">
         <f t="shared" si="3"/>
-        <v>-180157.72000000998</v>
-      </c>
-      <c r="J39" s="5">
-        <f t="shared" si="4"/>
         <v>-0.13918241656366656</v>
       </c>
-      <c r="K39">
-        <f t="shared" si="5"/>
+      <c r="K39" s="10">
+        <f>_xlfn.RANK.EQ($J39, $J$2:$J$52) +COUNTIF(J$2:J39,J39) -1</f>
         <v>49</v>
       </c>
       <c r="L39">
@@ -3480,15 +3487,15 @@
         <v>1680463.8699999901</v>
       </c>
       <c r="N39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-79036.1300000099</v>
       </c>
       <c r="O39" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-4.4919653310605226E-2</v>
       </c>
-      <c r="P39">
-        <f t="shared" si="8"/>
+      <c r="P39" s="10">
+        <f>_xlfn.RANK.EQ($O39, $O$2:$O$52) +COUNTIF(O$2:O39,O39) -1</f>
         <v>35</v>
       </c>
     </row>
@@ -3510,8 +3517,8 @@
         <f t="shared" si="1"/>
         <v>-2.1279773539092578E-2</v>
       </c>
-      <c r="F40">
-        <f t="shared" si="2"/>
+      <c r="F40" s="9">
+        <f>_xlfn.RANK.EQ($E40, $E$2:$E$52) +COUNTIF(E$2:E40,E40) -1</f>
         <v>29</v>
       </c>
       <c r="G40">
@@ -3521,15 +3528,15 @@
         <v>38095240.189999901</v>
       </c>
       <c r="I40">
+        <f t="shared" si="2"/>
+        <v>-1869659.8100000992</v>
+      </c>
+      <c r="J40" s="5">
         <f t="shared" si="3"/>
-        <v>-1869659.8100000992</v>
-      </c>
-      <c r="J40" s="5">
-        <f t="shared" si="4"/>
         <v>-4.6782546934937892E-2</v>
       </c>
-      <c r="K40">
-        <f t="shared" si="5"/>
+      <c r="K40" s="10">
+        <f>_xlfn.RANK.EQ($J40, $J$2:$J$52) +COUNTIF(J$2:J40,J40) -1</f>
         <v>30</v>
       </c>
       <c r="L40">
@@ -3539,15 +3546,15 @@
         <v>39606263.709999897</v>
       </c>
       <c r="N40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-610436.29000010341</v>
       </c>
       <c r="O40" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.5178676768608648E-2</v>
       </c>
-      <c r="P40">
-        <f t="shared" si="8"/>
+      <c r="P40" s="10">
+        <f>_xlfn.RANK.EQ($O40, $O$2:$O$52) +COUNTIF(O$2:O40,O40) -1</f>
         <v>21</v>
       </c>
     </row>
@@ -3569,8 +3576,8 @@
         <f t="shared" si="1"/>
         <v>-4.0110550149132493E-2</v>
       </c>
-      <c r="F41">
-        <f t="shared" si="2"/>
+      <c r="F41" s="9">
+        <f>_xlfn.RANK.EQ($E41, $E$2:$E$52) +COUNTIF(E$2:E41,E41) -1</f>
         <v>35</v>
       </c>
       <c r="G41">
@@ -3580,15 +3587,15 @@
         <v>4956043.6699999897</v>
       </c>
       <c r="I41">
+        <f t="shared" si="2"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="J41" s="5">
         <f t="shared" si="3"/>
-        <v>-133456.33000001032</v>
-      </c>
-      <c r="J41" s="5">
-        <f t="shared" si="4"/>
         <v>-2.6221894095689226E-2</v>
       </c>
-      <c r="K41">
-        <f t="shared" si="5"/>
+      <c r="K41" s="10">
+        <f>_xlfn.RANK.EQ($J41, $J$2:$J$52) +COUNTIF(J$2:J41,J41) -1</f>
         <v>18</v>
       </c>
       <c r="L41">
@@ -3598,15 +3605,15 @@
         <v>4717822.6500000004</v>
       </c>
       <c r="N41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-82077.349999999627</v>
       </c>
       <c r="O41" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.7099804162586642E-2</v>
       </c>
-      <c r="P41">
-        <f t="shared" si="8"/>
+      <c r="P41" s="10">
+        <f>_xlfn.RANK.EQ($O41, $O$2:$O$52) +COUNTIF(O$2:O41,O41) -1</f>
         <v>22</v>
       </c>
     </row>
@@ -3628,8 +3635,8 @@
         <f t="shared" si="1"/>
         <v>-2.2070943135841053E-4</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="2"/>
+      <c r="F42" s="9">
+        <f>_xlfn.RANK.EQ($E42, $E$2:$E$52) +COUNTIF(E$2:E42,E42) -1</f>
         <v>8</v>
       </c>
       <c r="G42">
@@ -3639,15 +3646,15 @@
         <v>196755033.31</v>
       </c>
       <c r="I42">
+        <f t="shared" si="2"/>
+        <v>-2375266.6899999976</v>
+      </c>
+      <c r="J42" s="5">
         <f t="shared" si="3"/>
-        <v>-2375266.6899999976</v>
-      </c>
-      <c r="J42" s="5">
-        <f t="shared" si="4"/>
         <v>-1.1928203241796942E-2</v>
       </c>
-      <c r="K42">
-        <f t="shared" si="5"/>
+      <c r="K42" s="10">
+        <f>_xlfn.RANK.EQ($J42, $J$2:$J$52) +COUNTIF(J$2:J42,J42) -1</f>
         <v>13</v>
       </c>
       <c r="L42">
@@ -3657,15 +3664,15 @@
         <v>199954563.74999899</v>
       </c>
       <c r="N42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-36.250001013278961</v>
       </c>
       <c r="O42" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.8129115815929696E-7</v>
       </c>
-      <c r="P42">
-        <f t="shared" si="8"/>
+      <c r="P42" s="10">
+        <f>_xlfn.RANK.EQ($O42, $O$2:$O$52) +COUNTIF(O$2:O42,O42) -1</f>
         <v>5</v>
       </c>
     </row>
@@ -3687,8 +3694,8 @@
         <f t="shared" si="1"/>
         <v>-2.0497353541313264E-2</v>
       </c>
-      <c r="F43">
-        <f t="shared" si="2"/>
+      <c r="F43" s="9">
+        <f>_xlfn.RANK.EQ($E43, $E$2:$E$52) +COUNTIF(E$2:E43,E43) -1</f>
         <v>28</v>
       </c>
       <c r="G43">
@@ -3698,15 +3705,15 @@
         <v>8171472.0199999996</v>
       </c>
       <c r="I43">
+        <f t="shared" si="2"/>
+        <v>-389327.98000000045</v>
+      </c>
+      <c r="J43" s="5">
         <f t="shared" si="3"/>
-        <v>-389327.98000000045</v>
-      </c>
-      <c r="J43" s="5">
-        <f t="shared" si="4"/>
         <v>-4.5477990374731388E-2</v>
       </c>
-      <c r="K43">
-        <f t="shared" si="5"/>
+      <c r="K43" s="10">
+        <f>_xlfn.RANK.EQ($J43, $J$2:$J$52) +COUNTIF(J$2:J43,J43) -1</f>
         <v>29</v>
       </c>
       <c r="L43">
@@ -3716,15 +3723,15 @@
         <v>8150982.5699999901</v>
       </c>
       <c r="N43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-346517.43000000995</v>
       </c>
       <c r="O43" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-4.0778750220654303E-2</v>
       </c>
-      <c r="P43">
-        <f t="shared" si="8"/>
+      <c r="P43" s="10">
+        <f>_xlfn.RANK.EQ($O43, $O$2:$O$52) +COUNTIF(O$2:O43,O43) -1</f>
         <v>34</v>
       </c>
     </row>
@@ -3746,8 +3753,8 @@
         <f t="shared" si="1"/>
         <v>-9.7760750186150751E-3</v>
       </c>
-      <c r="F44">
-        <f t="shared" si="2"/>
+      <c r="F44" s="9">
+        <f>_xlfn.RANK.EQ($E44, $E$2:$E$52) +COUNTIF(E$2:E44,E44) -1</f>
         <v>13</v>
       </c>
       <c r="G44">
@@ -3757,15 +3764,15 @@
         <v>30793711.48</v>
       </c>
       <c r="I44">
+        <f t="shared" si="2"/>
+        <v>-246988.51999999955</v>
+      </c>
+      <c r="J44" s="5">
         <f t="shared" si="3"/>
-        <v>-246988.51999999955</v>
-      </c>
-      <c r="J44" s="5">
-        <f t="shared" si="4"/>
         <v>-7.9569249404813532E-3</v>
       </c>
-      <c r="K44">
-        <f t="shared" si="5"/>
+      <c r="K44" s="10">
+        <f>_xlfn.RANK.EQ($J44, $J$2:$J$52) +COUNTIF(J$2:J44,J44) -1</f>
         <v>11</v>
       </c>
       <c r="L44">
@@ -3775,15 +3782,15 @@
         <v>31282141.25</v>
       </c>
       <c r="N44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-58.75</v>
       </c>
       <c r="O44" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.8780648419868168E-6</v>
       </c>
-      <c r="P44">
-        <f t="shared" si="8"/>
+      <c r="P44" s="10">
+        <f>_xlfn.RANK.EQ($O44, $O$2:$O$52) +COUNTIF(O$2:O44,O44) -1</f>
         <v>7</v>
       </c>
     </row>
@@ -3805,8 +3812,8 @@
         <f t="shared" si="1"/>
         <v>-1.287514194887851E-2</v>
       </c>
-      <c r="F45">
-        <f t="shared" si="2"/>
+      <c r="F45" s="9">
+        <f>_xlfn.RANK.EQ($E45, $E$2:$E$52) +COUNTIF(E$2:E45,E45) -1</f>
         <v>18</v>
       </c>
       <c r="G45">
@@ -3816,15 +3823,15 @@
         <v>54594953.959999897</v>
       </c>
       <c r="I45">
+        <f t="shared" si="2"/>
+        <v>-2197246.0400001034</v>
+      </c>
+      <c r="J45" s="5">
         <f t="shared" si="3"/>
-        <v>-2197246.0400001034</v>
-      </c>
-      <c r="J45" s="5">
-        <f t="shared" si="4"/>
         <v>-3.8689222111488959E-2</v>
       </c>
-      <c r="K45">
-        <f t="shared" si="5"/>
+      <c r="K45" s="10">
+        <f>_xlfn.RANK.EQ($J45, $J$2:$J$52) +COUNTIF(J$2:J45,J45) -1</f>
         <v>22</v>
       </c>
       <c r="L45">
@@ -3834,15 +3841,15 @@
         <v>55386549.6599999</v>
       </c>
       <c r="N45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-640550.34000010043</v>
       </c>
       <c r="O45" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.1432866237947358E-2</v>
       </c>
-      <c r="P45">
-        <f t="shared" si="8"/>
+      <c r="P45" s="10">
+        <f>_xlfn.RANK.EQ($O45, $O$2:$O$52) +COUNTIF(O$2:O45,O45) -1</f>
         <v>20</v>
       </c>
     </row>
@@ -3864,8 +3871,8 @@
         <f t="shared" si="1"/>
         <v>-3.0010420686993711E-3</v>
       </c>
-      <c r="F46">
-        <f t="shared" si="2"/>
+      <c r="F46" s="9">
+        <f>_xlfn.RANK.EQ($E46, $E$2:$E$52) +COUNTIF(E$2:E46,E46) -1</f>
         <v>9</v>
       </c>
       <c r="G46">
@@ -3875,15 +3882,15 @@
         <v>257402.90999999901</v>
       </c>
       <c r="I46">
+        <f t="shared" si="2"/>
+        <v>-8597.090000000986</v>
+      </c>
+      <c r="J46" s="5">
         <f t="shared" si="3"/>
-        <v>-8597.090000000986</v>
-      </c>
-      <c r="J46" s="5">
-        <f t="shared" si="4"/>
         <v>-3.2319887218048821E-2</v>
       </c>
-      <c r="K46">
-        <f t="shared" si="5"/>
+      <c r="K46" s="10">
+        <f>_xlfn.RANK.EQ($J46, $J$2:$J$52) +COUNTIF(J$2:J46,J46) -1</f>
         <v>19</v>
       </c>
       <c r="L46">
@@ -3893,15 +3900,15 @@
         <v>254753.15999999901</v>
       </c>
       <c r="N46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-12346.840000000986</v>
       </c>
       <c r="O46" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-4.6225533508053113E-2</v>
       </c>
-      <c r="P46">
-        <f t="shared" si="8"/>
+      <c r="P46" s="10">
+        <f>_xlfn.RANK.EQ($O46, $O$2:$O$52) +COUNTIF(O$2:O46,O46) -1</f>
         <v>36</v>
       </c>
     </row>
@@ -3923,8 +3930,8 @@
         <f t="shared" si="1"/>
         <v>-1.7435939690898361E-4</v>
       </c>
-      <c r="F47">
-        <f t="shared" si="2"/>
+      <c r="F47" s="9">
+        <f>_xlfn.RANK.EQ($E47, $E$2:$E$52) +COUNTIF(E$2:E47,E47) -1</f>
         <v>7</v>
       </c>
       <c r="G47">
@@ -3934,15 +3941,15 @@
         <v>73442541.659999996</v>
       </c>
       <c r="I47">
+        <f t="shared" si="2"/>
+        <v>-24458.340000003576</v>
+      </c>
+      <c r="J47" s="5">
         <f t="shared" si="3"/>
-        <v>-24458.340000003576</v>
-      </c>
-      <c r="J47" s="5">
-        <f t="shared" si="4"/>
         <v>-3.3291600310348285E-4</v>
       </c>
-      <c r="K47">
-        <f t="shared" si="5"/>
+      <c r="K47" s="10">
+        <f>_xlfn.RANK.EQ($J47, $J$2:$J$52) +COUNTIF(J$2:J47,J47) -1</f>
         <v>7</v>
       </c>
       <c r="L47">
@@ -3952,15 +3959,15 @@
         <v>75050829.179999903</v>
       </c>
       <c r="N47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-21970.820000097156</v>
       </c>
       <c r="O47" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-2.9266019117572752E-4</v>
       </c>
-      <c r="P47">
-        <f t="shared" si="8"/>
+      <c r="P47" s="10">
+        <f>_xlfn.RANK.EQ($O47, $O$2:$O$52) +COUNTIF(O$2:O47,O47) -1</f>
         <v>14</v>
       </c>
     </row>
@@ -3982,8 +3989,8 @@
         <f t="shared" si="1"/>
         <v>-3.1133192323107857E-2</v>
       </c>
-      <c r="F48">
-        <f t="shared" si="2"/>
+      <c r="F48" s="9">
+        <f>_xlfn.RANK.EQ($E48, $E$2:$E$52) +COUNTIF(E$2:E48,E48) -1</f>
         <v>32</v>
       </c>
       <c r="G48">
@@ -3993,15 +4000,15 @@
         <v>6922072.5599999996</v>
       </c>
       <c r="I48">
+        <f t="shared" si="2"/>
+        <v>-292627.44000000041</v>
+      </c>
+      <c r="J48" s="5">
         <f t="shared" si="3"/>
-        <v>-292627.44000000041</v>
-      </c>
-      <c r="J48" s="5">
-        <f t="shared" si="4"/>
         <v>-4.0559890224125802E-2</v>
       </c>
-      <c r="K48">
-        <f t="shared" si="5"/>
+      <c r="K48" s="10">
+        <f>_xlfn.RANK.EQ($J48, $J$2:$J$52) +COUNTIF(J$2:J48,J48) -1</f>
         <v>23</v>
       </c>
       <c r="L48">
@@ -4011,15 +4018,15 @@
         <v>6882350.23999999</v>
       </c>
       <c r="N48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-407449.76000001002</v>
       </c>
       <c r="O48" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-5.5893132870587676E-2</v>
       </c>
-      <c r="P48">
-        <f t="shared" si="8"/>
+      <c r="P48" s="10">
+        <f>_xlfn.RANK.EQ($O48, $O$2:$O$52) +COUNTIF(O$2:O48,O48) -1</f>
         <v>37</v>
       </c>
     </row>
@@ -4041,8 +4048,8 @@
         <f t="shared" si="1"/>
         <v>-1.8444360086767971E-2</v>
       </c>
-      <c r="F49">
-        <f t="shared" si="2"/>
+      <c r="F49" s="9">
+        <f>_xlfn.RANK.EQ($E49, $E$2:$E$52) +COUNTIF(E$2:E49,E49) -1</f>
         <v>25</v>
       </c>
       <c r="G49">
@@ -4052,34 +4059,34 @@
         <v>95466.880000000005</v>
       </c>
       <c r="I49">
+        <f t="shared" si="2"/>
+        <v>-7133.1199999999953</v>
+      </c>
+      <c r="J49" s="5">
         <f t="shared" si="3"/>
-        <v>-7133.1199999999953</v>
-      </c>
-      <c r="J49" s="5">
+        <v>-6.9523586744639335E-2</v>
+      </c>
+      <c r="K49" s="10">
+        <f>_xlfn.RANK.EQ($J49, $J$2:$J$52) +COUNTIF(J$2:J49,J49) -1</f>
+        <v>39</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
         <f t="shared" si="4"/>
-        <v>-6.9523586744639335E-2</v>
-      </c>
-      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="O49" s="5">
         <f t="shared" si="5"/>
-        <v>39</v>
-      </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-      <c r="M49">
-        <v>0</v>
-      </c>
-      <c r="N49">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O49" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P49">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="P49" s="10">
+        <f>_xlfn.RANK.EQ($O49, $O$2:$O$52) +COUNTIF(O$2:O49,O49) -1</f>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -4100,9 +4107,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F50">
-        <f t="shared" si="2"/>
-        <v>2</v>
+      <c r="F50" s="9">
+        <f>_xlfn.RANK.EQ($E50, $E$2:$E$52) +COUNTIF(E$2:E50,E50) -1</f>
+        <v>5</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -4111,16 +4118,16 @@
         <v>859100</v>
       </c>
       <c r="I50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J50" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <f t="shared" si="5"/>
-        <v>1</v>
+      <c r="K50" s="10">
+        <f>_xlfn.RANK.EQ($J50, $J$2:$J$52) +COUNTIF(J$2:J50,J50) -1</f>
+        <v>4</v>
       </c>
       <c r="L50">
         <v>843200</v>
@@ -4129,16 +4136,16 @@
         <v>843200</v>
       </c>
       <c r="N50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O50" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P50">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P50" s="10">
+        <f>_xlfn.RANK.EQ($O50, $O$2:$O$52) +COUNTIF(O$2:O50,O50) -1</f>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -4159,8 +4166,8 @@
         <f t="shared" si="1"/>
         <v>-1.2785255822058129E-2</v>
       </c>
-      <c r="F51">
-        <f t="shared" si="2"/>
+      <c r="F51" s="9">
+        <f>_xlfn.RANK.EQ($E51, $E$2:$E$52) +COUNTIF(E$2:E51,E51) -1</f>
         <v>17</v>
       </c>
       <c r="G51">
@@ -4170,15 +4177,15 @@
         <v>8599059.6199999992</v>
       </c>
       <c r="I51">
+        <f t="shared" si="2"/>
+        <v>-326440.38000000082</v>
+      </c>
+      <c r="J51" s="5">
         <f t="shared" si="3"/>
-        <v>-326440.38000000082</v>
-      </c>
-      <c r="J51" s="5">
-        <f t="shared" si="4"/>
         <v>-3.6573903982970231E-2</v>
       </c>
-      <c r="K51">
-        <f t="shared" si="5"/>
+      <c r="K51" s="10">
+        <f>_xlfn.RANK.EQ($J51, $J$2:$J$52) +COUNTIF(J$2:J51,J51) -1</f>
         <v>21</v>
       </c>
       <c r="L51">
@@ -4188,15 +4195,15 @@
         <v>8735843.3100000005</v>
       </c>
       <c r="N51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-98056.689999999478</v>
       </c>
       <c r="O51" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-1.1100045280114048E-2</v>
       </c>
-      <c r="P51">
-        <f t="shared" si="8"/>
+      <c r="P51" s="10">
+        <f>_xlfn.RANK.EQ($O51, $O$2:$O$52) +COUNTIF(O$2:O51,O51) -1</f>
         <v>19</v>
       </c>
     </row>
@@ -4218,8 +4225,8 @@
         <f t="shared" si="1"/>
         <v>-8.009596083231342E-2</v>
       </c>
-      <c r="F52">
-        <f t="shared" si="2"/>
+      <c r="F52" s="9">
+        <f>_xlfn.RANK.EQ($E52, $E$2:$E$52) +COUNTIF(E$2:E52,E52) -1</f>
         <v>45</v>
       </c>
       <c r="G52">
@@ -4229,15 +4236,15 @@
         <v>2204672.88</v>
       </c>
       <c r="I52">
+        <f t="shared" si="2"/>
+        <v>-236027.12000000011</v>
+      </c>
+      <c r="J52" s="5">
         <f t="shared" si="3"/>
-        <v>-236027.12000000011</v>
-      </c>
-      <c r="J52" s="5">
-        <f t="shared" si="4"/>
         <v>-9.6704683082722218E-2</v>
       </c>
-      <c r="K52">
-        <f t="shared" si="5"/>
+      <c r="K52" s="10">
+        <f>_xlfn.RANK.EQ($J52, $J$2:$J$52) +COUNTIF(J$2:J52,J52) -1</f>
         <v>43</v>
       </c>
       <c r="L52">
@@ -4247,15 +4254,15 @@
         <v>2056835.26</v>
       </c>
       <c r="N52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-264764.74</v>
       </c>
       <c r="O52" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-0.11404408166781529</v>
       </c>
-      <c r="P52">
-        <f t="shared" si="8"/>
+      <c r="P52" s="10">
+        <f>_xlfn.RANK.EQ($O52, $O$2:$O$52) +COUNTIF(O$2:O52,O52) -1</f>
         <v>46</v>
       </c>
     </row>
@@ -4292,11 +4299,11 @@
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f t="shared" ref="C56:D61" si="9">VLOOKUP($A56, $A$2:$P$52, MATCH(C$55, $A$1:$P$1, 0), FALSE)</f>
+        <f t="shared" ref="C56:D61" si="6">VLOOKUP($A56, $A$2:$P$52, MATCH(C$55, $A$1:$P$1, 0), FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4305,15 +4312,15 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="10">VLOOKUP($A57, $A$2:$P$52, MATCH(B$55, $A$1:$P$1, 0), FALSE)</f>
+        <f t="shared" ref="B57:B61" si="7">VLOOKUP($A57, $A$2:$P$52, MATCH(B$55, $A$1:$P$1, 0), FALSE)</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4322,15 +4329,15 @@
         <v>32</v>
       </c>
       <c r="B58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4339,15 +4346,15 @@
         <v>38</v>
       </c>
       <c r="B59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4356,15 +4363,15 @@
         <v>39</v>
       </c>
       <c r="B60">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4373,15 +4380,15 @@
         <v>55</v>
       </c>
       <c r="B61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4413,11 +4420,11 @@
         <v>-36209.630000000005</v>
       </c>
       <c r="C65">
-        <f t="shared" ref="C65:D70" si="11">VLOOKUP($A65, $A$2:$P$52, MATCH(C$64, $A$1:$P$1, 0), FALSE)</f>
+        <f t="shared" ref="C65:D70" si="8">VLOOKUP($A65, $A$2:$P$52, MATCH(C$64, $A$1:$P$1, 0), FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D65">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4426,15 +4433,15 @@
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="12">VLOOKUP($A66, $A$2:$P$52, MATCH($B$64, $A$1:$P$1, 0), FALSE)</f>
+        <f t="shared" ref="B66:B70" si="9">VLOOKUP($A66, $A$2:$P$52, MATCH($B$64, $A$1:$P$1, 0), FALSE)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4443,15 +4450,15 @@
         <v>32</v>
       </c>
       <c r="B67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4460,15 +4467,15 @@
         <v>38</v>
       </c>
       <c r="B68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4477,15 +4484,15 @@
         <v>39</v>
       </c>
       <c r="B69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4494,15 +4501,15 @@
         <v>55</v>
       </c>
       <c r="B70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4534,11 +4541,11 @@
         <v>-36209.630000000005</v>
       </c>
       <c r="C74">
-        <f t="shared" ref="C74:D79" si="13">VLOOKUP($A74, $A$2:$P$52, MATCH(C$73, $A$1:$P$1, 0), FALSE)</f>
+        <f t="shared" ref="C74:D79" si="10">VLOOKUP($A74, $A$2:$P$52, MATCH(C$73, $A$1:$P$1, 0), FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D74">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4547,15 +4554,15 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="14">VLOOKUP($A75, $A$2:$P$52, MATCH(B$73, $A$1:$P$1, 0), FALSE)</f>
+        <f t="shared" ref="B75:B79" si="11">VLOOKUP($A75, $A$2:$P$52, MATCH(B$73, $A$1:$P$1, 0), FALSE)</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4564,15 +4571,15 @@
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4581,15 +4588,15 @@
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4598,15 +4605,15 @@
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4615,29 +4622,29 @@
         <v>55</v>
       </c>
       <c r="B79">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>71</v>
       </c>
@@ -4645,7 +4652,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>73</v>
       </c>
@@ -4658,7 +4665,7 @@
         <v>385908.52</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>74</v>
       </c>
@@ -4671,7 +4678,7 @@
         <v>427758.64</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>75</v>
       </c>
@@ -4684,17 +4691,20 @@
         <v>445114.28999999899</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I88" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -4709,8 +4719,12 @@
       <c r="F89" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I89">
+        <f>MATCH($B$89, $F$2:$F$52, 0)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B90" s="7" t="s">
         <v>0</v>
       </c>
@@ -4729,37 +4743,112 @@
       <c r="G90" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I90">
+        <f>MATCH($A91&amp;"_rank", $A$1:$P$1, 0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>73</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="G91" s="5"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B91" t="str">
+        <f>_xlfn.XLOOKUP($B$89, $F$2:$F$52, $A$2:$A$52)</f>
+        <v>Debt Service</v>
+      </c>
+      <c r="C91" s="5">
+        <f>_xlfn.XLOOKUP($B91, $A$2:$A$52, $E$2:$E$52)</f>
+        <v>3.1837408866824991E-3</v>
+      </c>
+      <c r="D91" t="str">
+        <f>_xlfn.XLOOKUP($D$89, $F$2:$F$52, $A$2:$A$52)</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="E91" s="5">
+        <f>_xlfn.XLOOKUP($D91, $A$2:$A$52, $E$2:$E$52)</f>
+        <v>0</v>
+      </c>
+      <c r="F91" t="str">
+        <f>_xlfn.XLOOKUP($F$89, $F$2:$F$52, $A$2:$A$52)</f>
+        <v>Information Technology Service</v>
+      </c>
+      <c r="G91" s="5">
+        <f>_xlfn.XLOOKUP($F91, $A$2:$A$52, $E$2:$E$52)</f>
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <f>INDEX($A1:$P52, MATCH($B$89, $F$2:$F$52, 0), MATCH($A91&amp;"_rank", $A$1:$P$1, 0))</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="G92" s="5"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B92" t="str">
+        <f>_xlfn.XLOOKUP($B$89, $K$2:$K$52, $A$2:$A$52)</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C92" s="5">
+        <f>_xlfn.XLOOKUP($B92, $A$2:$A$52, $J$2:$J$52)</f>
+        <v>0</v>
+      </c>
+      <c r="D92" t="str">
+        <f>_xlfn.XLOOKUP($D$89, $K$2:$K$52, $A$2:$A$52)</f>
+        <v>Information Technology Service</v>
+      </c>
+      <c r="E92" s="5">
+        <f t="shared" ref="E92:E93" si="12">_xlfn.XLOOKUP($D92, $A$2:$A$52, $J$2:$J$52)</f>
+        <v>0</v>
+      </c>
+      <c r="F92" t="str">
+        <f>_xlfn.XLOOKUP($F$89, $K$2:$K$52, $A$2:$A$52)</f>
+        <v>Medical Examiner</v>
+      </c>
+      <c r="G92" s="5">
+        <f>_xlfn.XLOOKUP($F92, $A$2:$A$52, $J$2:$J$52)</f>
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <f>MATCH($A91&amp;"_rank", $A$1:$P$1, 0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>75</v>
       </c>
-      <c r="C93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="G93" s="5"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B93" t="str">
+        <f>_xlfn.XLOOKUP($B$89, $P$2:$P$52, $A$2:$A$52)</f>
+        <v>Information Technology Service</v>
+      </c>
+      <c r="C93" s="5">
+        <f>_xlfn.XLOOKUP($B93, $A$2:$A$52, $O$2:$O$52)</f>
+        <v>0</v>
+      </c>
+      <c r="D93" t="str">
+        <f>_xlfn.XLOOKUP($D$89, $P$2:$P$52, $A$2:$A$52)</f>
+        <v>Medical Examiner</v>
+      </c>
+      <c r="E93" s="5">
+        <f>_xlfn.XLOOKUP($D93, $A$2:$A$52, $O$2:$O$52)</f>
+        <v>0</v>
+      </c>
+      <c r="F93" t="str">
+        <f>_xlfn.XLOOKUP($F$89, $P$2:$P$52, $A$2:$A$52)</f>
+        <v>Soil and Water Conservation</v>
+      </c>
+      <c r="G93" s="5">
+        <f t="shared" ref="G92:G93" si="13">_xlfn.XLOOKUP($F93, $A$2:$A$52, $O$2:$O$52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
updated answers based on walkthrough
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick Nash\Documents\nss-data-analytics-08\projects\budget_lookups-thenicknash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1443D513-3261-445F-BF1A-EEEF0E69AA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2171D7B-8536-4AE1-B265-C2C8E3B93284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -308,8 +308,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -825,8 +826,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1184,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="I88" sqref="I88:I92"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,8 +1274,8 @@
         <v>-4.3170750765267295E-2</v>
       </c>
       <c r="F2" s="9">
-        <f>_xlfn.RANK.EQ($E2, $E$2:$E$52) +COUNTIF(E$2:E2,E2) -1</f>
-        <v>38</v>
+        <f>_xlfn.RANK.EQ($E2, $E$2:$E$52, 1) +COUNTIF(E$2:E2,E2) -1</f>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>382685200</v>
@@ -1290,9 +1291,9 @@
         <f>IFERROR(I2 / G2, 0)</f>
         <v>-9.4972027086493035E-2</v>
       </c>
-      <c r="K2" s="10">
-        <f>_xlfn.RANK.EQ($J2, $J$2:$J$52) +COUNTIF(J$2:J2,J2) -1</f>
-        <v>42</v>
+      <c r="K2" s="9">
+        <f>_xlfn.RANK.EQ($J2, $J$2:$J$52, 1) +COUNTIF(J$2:J2,J2) -1</f>
+        <v>10</v>
       </c>
       <c r="L2">
         <v>376548600</v>
@@ -1308,9 +1309,9 @@
         <f>IFERROR(N2/L2, 0)</f>
         <v>-5.6484362894991494E-2</v>
       </c>
-      <c r="P2" s="10">
-        <f>_xlfn.RANK.EQ($O2, $O$2:$O$52) +COUNTIF(O$2:O2,O2) -1</f>
-        <v>38</v>
+      <c r="P2" s="9">
+        <f>_xlfn.RANK.EQ($O2, $O$2:$O$52, 1) +COUNTIF(O$2:O2,O2) -1</f>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1332,8 +1333,8 @@
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3" s="9">
-        <f>_xlfn.RANK.EQ($E3, $E$2:$E$52) +COUNTIF(E$2:E3,E3) -1</f>
-        <v>30</v>
+        <f>_xlfn.RANK.EQ($E3, $E$2:$E$52, 1) +COUNTIF(E$2:E3,E3) -1</f>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>334800</v>
@@ -1349,9 +1350,9 @@
         <f t="shared" ref="J3:J52" si="3">IFERROR(I3 / G3, 0)</f>
         <v>-6.6804928315415249E-2</v>
       </c>
-      <c r="K3" s="10">
-        <f>_xlfn.RANK.EQ($J3, $J$2:$J$52) +COUNTIF(J$2:J3,J3) -1</f>
-        <v>38</v>
+      <c r="K3" s="9">
+        <f>_xlfn.RANK.EQ($J3, $J$2:$J$52, 1) +COUNTIF(J$2:J3,J3) -1</f>
+        <v>14</v>
       </c>
       <c r="L3">
         <v>322700</v>
@@ -1367,9 +1368,9 @@
         <f t="shared" ref="O3:O52" si="5">IFERROR(N3/L3, 0)</f>
         <v>-1.3540749922529313E-3</v>
       </c>
-      <c r="P3" s="10">
-        <f>_xlfn.RANK.EQ($O3, $O$2:$O$52) +COUNTIF(O$2:O3,O3) -1</f>
-        <v>15</v>
+      <c r="P3" s="9">
+        <f>_xlfn.RANK.EQ($O3, $O$2:$O$52, 1) +COUNTIF(O$2:O3,O3) -1</f>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1391,8 +1392,8 @@
         <v>-4.9327413275443007E-3</v>
       </c>
       <c r="F4" s="9">
-        <f>_xlfn.RANK.EQ($E4, $E$2:$E$52) +COUNTIF(E$2:E4,E4) -1</f>
-        <v>10</v>
+        <f>_xlfn.RANK.EQ($E4, $E$2:$E$52, 1) +COUNTIF(E$2:E4,E4) -1</f>
+        <v>42</v>
       </c>
       <c r="G4">
         <v>3652300</v>
@@ -1408,9 +1409,9 @@
         <f t="shared" si="3"/>
         <v>-1.7141743558856015E-2</v>
       </c>
-      <c r="K4" s="10">
-        <f>_xlfn.RANK.EQ($J4, $J$2:$J$52) +COUNTIF(J$2:J4,J4) -1</f>
-        <v>16</v>
+      <c r="K4" s="9">
+        <f>_xlfn.RANK.EQ($J4, $J$2:$J$52, 1) +COUNTIF(J$2:J4,J4) -1</f>
+        <v>36</v>
       </c>
       <c r="L4">
         <v>3662400</v>
@@ -1426,9 +1427,9 @@
         <f t="shared" si="5"/>
         <v>-2.6599210899959033E-2</v>
       </c>
-      <c r="P4" s="10">
-        <f>_xlfn.RANK.EQ($O4, $O$2:$O$52) +COUNTIF(O$2:O4,O4) -1</f>
-        <v>27</v>
+      <c r="P4" s="9">
+        <f>_xlfn.RANK.EQ($O4, $O$2:$O$52, 1) +COUNTIF(O$2:O4,O4) -1</f>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1450,8 +1451,8 @@
         <v>-9.4273968477453174E-2</v>
       </c>
       <c r="F5" s="9">
-        <f>_xlfn.RANK.EQ($E5, $E$2:$E$52) +COUNTIF(E$2:E5,E5) -1</f>
-        <v>48</v>
+        <f>_xlfn.RANK.EQ($E5, $E$2:$E$52, 1) +COUNTIF(E$2:E5,E5) -1</f>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>7968300</v>
@@ -1467,9 +1468,9 @@
         <f t="shared" si="3"/>
         <v>-0.118932605449092</v>
       </c>
-      <c r="K5" s="10">
-        <f>_xlfn.RANK.EQ($J5, $J$2:$J$52) +COUNTIF(J$2:J5,J5) -1</f>
-        <v>47</v>
+      <c r="K5" s="9">
+        <f>_xlfn.RANK.EQ($J5, $J$2:$J$52, 1) +COUNTIF(J$2:J5,J5) -1</f>
+        <v>5</v>
       </c>
       <c r="L5">
         <v>7759600</v>
@@ -1485,9 +1486,9 @@
         <f t="shared" si="5"/>
         <v>-3.3800336357544182E-2</v>
       </c>
-      <c r="P5" s="10">
-        <f>_xlfn.RANK.EQ($O5, $O$2:$O$52) +COUNTIF(O$2:O5,O5) -1</f>
-        <v>30</v>
+      <c r="P5" s="9">
+        <f>_xlfn.RANK.EQ($O5, $O$2:$O$52, 1) +COUNTIF(O$2:O5,O5) -1</f>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1509,8 +1510,8 @@
         <v>-5.7149963352064452E-2</v>
       </c>
       <c r="F6" s="9">
-        <f>_xlfn.RANK.EQ($E6, $E$2:$E$52) +COUNTIF(E$2:E6,E6) -1</f>
-        <v>41</v>
+        <f>_xlfn.RANK.EQ($E6, $E$2:$E$52, 1) +COUNTIF(E$2:E6,E6) -1</f>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -1526,9 +1527,9 @@
         <f t="shared" si="3"/>
         <v>-1.7301283547257551E-3</v>
       </c>
-      <c r="K6" s="10">
-        <f>_xlfn.RANK.EQ($J6, $J$2:$J$52) +COUNTIF(J$2:J6,J6) -1</f>
-        <v>8</v>
+      <c r="K6" s="9">
+        <f>_xlfn.RANK.EQ($J6, $J$2:$J$52, 1) +COUNTIF(J$2:J6,J6) -1</f>
+        <v>44</v>
       </c>
       <c r="L6">
         <v>445200</v>
@@ -1544,9 +1545,9 @@
         <f t="shared" si="5"/>
         <v>-1.925202156356929E-4</v>
       </c>
-      <c r="P6" s="10">
-        <f>_xlfn.RANK.EQ($O6, $O$2:$O$52) +COUNTIF(O$2:O6,O6) -1</f>
-        <v>13</v>
+      <c r="P6" s="9">
+        <f>_xlfn.RANK.EQ($O6, $O$2:$O$52, 1) +COUNTIF(O$2:O6,O6) -1</f>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1568,8 +1569,8 @@
         <v>-0.11502817362571344</v>
       </c>
       <c r="F7" s="9">
-        <f>_xlfn.RANK.EQ($E7, $E$2:$E$52) +COUNTIF(E$2:E7,E7) -1</f>
-        <v>50</v>
+        <f>_xlfn.RANK.EQ($E7, $E$2:$E$52, 1) +COUNTIF(E$2:E7,E7) -1</f>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>3390900</v>
@@ -1585,9 +1586,9 @@
         <f t="shared" si="3"/>
         <v>-0.10009631366303927</v>
       </c>
-      <c r="K7" s="10">
-        <f>_xlfn.RANK.EQ($J7, $J$2:$J$52) +COUNTIF(J$2:J7,J7) -1</f>
-        <v>44</v>
+      <c r="K7" s="9">
+        <f>_xlfn.RANK.EQ($J7, $J$2:$J$52, 1) +COUNTIF(J$2:J7,J7) -1</f>
+        <v>8</v>
       </c>
       <c r="L7">
         <v>3345200</v>
@@ -1603,9 +1604,9 @@
         <f t="shared" si="5"/>
         <v>-0.11920361114432618</v>
       </c>
-      <c r="P7" s="10">
-        <f>_xlfn.RANK.EQ($O7, $O$2:$O$52) +COUNTIF(O$2:O7,O7) -1</f>
-        <v>48</v>
+      <c r="P7" s="9">
+        <f>_xlfn.RANK.EQ($O7, $O$2:$O$52, 1) +COUNTIF(O$2:O7,O7) -1</f>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1627,8 +1628,8 @@
         <v>-0.15235918433091292</v>
       </c>
       <c r="F8" s="9">
-        <f>_xlfn.RANK.EQ($E8, $E$2:$E$52) +COUNTIF(E$2:E8,E8) -1</f>
-        <v>51</v>
+        <f>_xlfn.RANK.EQ($E8, $E$2:$E$52, 1) +COUNTIF(E$2:E8,E8) -1</f>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>1590700</v>
@@ -1644,9 +1645,9 @@
         <f t="shared" si="3"/>
         <v>-0.13000189224870184</v>
       </c>
-      <c r="K8" s="10">
-        <f>_xlfn.RANK.EQ($J8, $J$2:$J$52) +COUNTIF(J$2:J8,J8) -1</f>
-        <v>48</v>
+      <c r="K8" s="9">
+        <f>_xlfn.RANK.EQ($J8, $J$2:$J$52, 1) +COUNTIF(J$2:J8,J8) -1</f>
+        <v>4</v>
       </c>
       <c r="L8">
         <v>1579300</v>
@@ -1662,9 +1663,9 @@
         <f t="shared" si="5"/>
         <v>-0.15295680364719175</v>
       </c>
-      <c r="P8" s="10">
-        <f>_xlfn.RANK.EQ($O8, $O$2:$O$52) +COUNTIF(O$2:O8,O8) -1</f>
-        <v>50</v>
+      <c r="P8" s="9">
+        <f>_xlfn.RANK.EQ($O8, $O$2:$O$52, 1) +COUNTIF(O$2:O8,O8) -1</f>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1686,8 +1687,8 @@
         <v>-4.2417130511048909E-2</v>
       </c>
       <c r="F9" s="9">
-        <f>_xlfn.RANK.EQ($E9, $E$2:$E$52) +COUNTIF(E$2:E9,E9) -1</f>
-        <v>36</v>
+        <f>_xlfn.RANK.EQ($E9, $E$2:$E$52, 1) +COUNTIF(E$2:E9,E9) -1</f>
+        <v>16</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -1703,9 +1704,9 @@
         <f t="shared" si="3"/>
         <v>-0.10336567542917005</v>
       </c>
-      <c r="K9" s="10">
-        <f>_xlfn.RANK.EQ($J9, $J$2:$J$52) +COUNTIF(J$2:J9,J9) -1</f>
-        <v>45</v>
+      <c r="K9" s="9">
+        <f>_xlfn.RANK.EQ($J9, $J$2:$J$52, 1) +COUNTIF(J$2:J9,J9) -1</f>
+        <v>7</v>
       </c>
       <c r="L9">
         <v>10790500</v>
@@ -1721,9 +1722,9 @@
         <f t="shared" si="5"/>
         <v>-7.3852043000788653E-2</v>
       </c>
-      <c r="P9" s="10">
-        <f>_xlfn.RANK.EQ($O9, $O$2:$O$52) +COUNTIF(O$2:O9,O9) -1</f>
-        <v>43</v>
+      <c r="P9" s="9">
+        <f>_xlfn.RANK.EQ($O9, $O$2:$O$52, 1) +COUNTIF(O$2:O9,O9) -1</f>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1745,8 +1746,8 @@
         <v>-8.1681998646514792E-2</v>
       </c>
       <c r="F10" s="9">
-        <f>_xlfn.RANK.EQ($E10, $E$2:$E$52) +COUNTIF(E$2:E10,E10) -1</f>
-        <v>46</v>
+        <f>_xlfn.RANK.EQ($E10, $E$2:$E$52, 1) +COUNTIF(E$2:E10,E10) -1</f>
+        <v>6</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -1762,9 +1763,9 @@
         <f t="shared" si="3"/>
         <v>-5.5113408723747932E-2</v>
       </c>
-      <c r="K10" s="10">
-        <f>_xlfn.RANK.EQ($J10, $J$2:$J$52) +COUNTIF(J$2:J10,J10) -1</f>
-        <v>35</v>
+      <c r="K10" s="9">
+        <f>_xlfn.RANK.EQ($J10, $J$2:$J$52, 1) +COUNTIF(J$2:J10,J10) -1</f>
+        <v>17</v>
       </c>
       <c r="L10">
         <v>487500</v>
@@ -1780,9 +1781,9 @@
         <f t="shared" si="5"/>
         <v>-1.883298461538465E-2</v>
       </c>
-      <c r="P10" s="10">
-        <f>_xlfn.RANK.EQ($O10, $O$2:$O$52) +COUNTIF(O$2:O10,O10) -1</f>
-        <v>23</v>
+      <c r="P10" s="9">
+        <f>_xlfn.RANK.EQ($O10, $O$2:$O$52, 1) +COUNTIF(O$2:O10,O10) -1</f>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1804,8 +1805,8 @@
         <v>0</v>
       </c>
       <c r="F11" s="9">
-        <f>_xlfn.RANK.EQ($E11, $E$2:$E$52) +COUNTIF(E$2:E11,E11) -1</f>
-        <v>2</v>
+        <f>_xlfn.RANK.EQ($E11, $E$2:$E$52, 1) +COUNTIF(E$2:E11,E11) -1</f>
+        <v>47</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1821,9 +1822,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K11" s="10">
-        <f>_xlfn.RANK.EQ($J11, $J$2:$J$52) +COUNTIF(J$2:J11,J11) -1</f>
-        <v>1</v>
+      <c r="K11" s="9">
+        <f>_xlfn.RANK.EQ($J11, $J$2:$J$52, 1) +COUNTIF(J$2:J11,J11) -1</f>
+        <v>48</v>
       </c>
       <c r="L11">
         <v>375000</v>
@@ -1839,9 +1840,9 @@
         <f t="shared" si="5"/>
         <v>-0.82994157333333329</v>
       </c>
-      <c r="P11" s="10">
-        <f>_xlfn.RANK.EQ($O11, $O$2:$O$52) +COUNTIF(O$2:O11,O11) -1</f>
-        <v>51</v>
+      <c r="P11" s="9">
+        <f>_xlfn.RANK.EQ($O11, $O$2:$O$52, 1) +COUNTIF(O$2:O11,O11) -1</f>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1863,8 +1864,8 @@
         <v>-5.0060657805601608E-2</v>
       </c>
       <c r="F12" s="9">
-        <f>_xlfn.RANK.EQ($E12, $E$2:$E$52) +COUNTIF(E$2:E12,E12) -1</f>
-        <v>39</v>
+        <f>_xlfn.RANK.EQ($E12, $E$2:$E$52, 1) +COUNTIF(E$2:E12,E12) -1</f>
+        <v>13</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -1880,9 +1881,9 @@
         <f t="shared" si="3"/>
         <v>-0.10527708280146378</v>
       </c>
-      <c r="K12" s="10">
-        <f>_xlfn.RANK.EQ($J12, $J$2:$J$52) +COUNTIF(J$2:J12,J12) -1</f>
-        <v>46</v>
+      <c r="K12" s="9">
+        <f>_xlfn.RANK.EQ($J12, $J$2:$J$52, 1) +COUNTIF(J$2:J12,J12) -1</f>
+        <v>6</v>
       </c>
       <c r="L12">
         <v>4677800</v>
@@ -1898,9 +1899,9 @@
         <f t="shared" si="5"/>
         <v>-6.5433934755654441E-2</v>
       </c>
-      <c r="P12" s="10">
-        <f>_xlfn.RANK.EQ($O12, $O$2:$O$52) +COUNTIF(O$2:O12,O12) -1</f>
-        <v>42</v>
+      <c r="P12" s="9">
+        <f>_xlfn.RANK.EQ($O12, $O$2:$O$52, 1) +COUNTIF(O$2:O12,O12) -1</f>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1922,8 +1923,8 @@
         <v>-1.2912833886247806E-2</v>
       </c>
       <c r="F13" s="9">
-        <f>_xlfn.RANK.EQ($E13, $E$2:$E$52) +COUNTIF(E$2:E13,E13) -1</f>
-        <v>19</v>
+        <f>_xlfn.RANK.EQ($E13, $E$2:$E$52, 1) +COUNTIF(E$2:E13,E13) -1</f>
+        <v>33</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -1939,9 +1940,9 @@
         <f t="shared" si="3"/>
         <v>-5.0552253482656594E-2</v>
       </c>
-      <c r="K13" s="10">
-        <f>_xlfn.RANK.EQ($J13, $J$2:$J$52) +COUNTIF(J$2:J13,J13) -1</f>
-        <v>34</v>
+      <c r="K13" s="9">
+        <f>_xlfn.RANK.EQ($J13, $J$2:$J$52, 1) +COUNTIF(J$2:J13,J13) -1</f>
+        <v>18</v>
       </c>
       <c r="L13">
         <v>6207300</v>
@@ -1957,9 +1958,9 @@
         <f t="shared" si="5"/>
         <v>-2.4217184605222895E-2</v>
       </c>
-      <c r="P13" s="10">
-        <f>_xlfn.RANK.EQ($O13, $O$2:$O$52) +COUNTIF(O$2:O13,O13) -1</f>
-        <v>25</v>
+      <c r="P13" s="9">
+        <f>_xlfn.RANK.EQ($O13, $O$2:$O$52, 1) +COUNTIF(O$2:O13,O13) -1</f>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1981,8 +1982,8 @@
         <v>-1.3637949218750009E-2</v>
       </c>
       <c r="F14" s="9">
-        <f>_xlfn.RANK.EQ($E14, $E$2:$E$52) +COUNTIF(E$2:E14,E14) -1</f>
-        <v>22</v>
+        <f>_xlfn.RANK.EQ($E14, $E$2:$E$52, 1) +COUNTIF(E$2:E14,E14) -1</f>
+        <v>30</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -1998,9 +1999,9 @@
         <f t="shared" si="3"/>
         <v>-1.1492968897266765E-2</v>
       </c>
-      <c r="K14" s="10">
-        <f>_xlfn.RANK.EQ($J14, $J$2:$J$52) +COUNTIF(J$2:J14,J14) -1</f>
-        <v>12</v>
+      <c r="K14" s="9">
+        <f>_xlfn.RANK.EQ($J14, $J$2:$J$52, 1) +COUNTIF(J$2:J14,J14) -1</f>
+        <v>40</v>
       </c>
       <c r="L14">
         <v>526200</v>
@@ -2016,9 +2017,9 @@
         <f t="shared" si="5"/>
         <v>-4.0308095781071827E-2</v>
       </c>
-      <c r="P14" s="10">
-        <f>_xlfn.RANK.EQ($O14, $O$2:$O$52) +COUNTIF(O$2:O14,O14) -1</f>
-        <v>33</v>
+      <c r="P14" s="9">
+        <f>_xlfn.RANK.EQ($O14, $O$2:$O$52, 1) +COUNTIF(O$2:O14,O14) -1</f>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2040,8 +2041,8 @@
         <v>3.1837408866824991E-3</v>
       </c>
       <c r="F15" s="9">
-        <f>_xlfn.RANK.EQ($E15, $E$2:$E$52) +COUNTIF(E$2:E15,E15) -1</f>
-        <v>1</v>
+        <f>_xlfn.RANK.EQ($E15, $E$2:$E$52, 1) +COUNTIF(E$2:E15,E15) -1</f>
+        <v>51</v>
       </c>
       <c r="G15">
         <v>184167800</v>
@@ -2057,9 +2058,9 @@
         <f t="shared" si="3"/>
         <v>-4.4532273014072019E-2</v>
       </c>
-      <c r="K15" s="10">
-        <f>_xlfn.RANK.EQ($J15, $J$2:$J$52) +COUNTIF(J$2:J15,J15) -1</f>
-        <v>28</v>
+      <c r="K15" s="9">
+        <f>_xlfn.RANK.EQ($J15, $J$2:$J$52, 1) +COUNTIF(J$2:J15,J15) -1</f>
+        <v>24</v>
       </c>
       <c r="L15">
         <v>188953500</v>
@@ -2075,9 +2076,9 @@
         <f t="shared" si="5"/>
         <v>-2.3829085727446114E-2</v>
       </c>
-      <c r="P15" s="10">
-        <f>_xlfn.RANK.EQ($O15, $O$2:$O$52) +COUNTIF(O$2:O15,O15) -1</f>
-        <v>24</v>
+      <c r="P15" s="9">
+        <f>_xlfn.RANK.EQ($O15, $O$2:$O$52, 1) +COUNTIF(O$2:O15,O15) -1</f>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -2099,8 +2100,8 @@
         <v>-1.1850188616360429E-2</v>
       </c>
       <c r="F16" s="9">
-        <f>_xlfn.RANK.EQ($E16, $E$2:$E$52) +COUNTIF(E$2:E16,E16) -1</f>
-        <v>15</v>
+        <f>_xlfn.RANK.EQ($E16, $E$2:$E$52, 1) +COUNTIF(E$2:E16,E16) -1</f>
+        <v>37</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -2116,9 +2117,9 @@
         <f t="shared" si="3"/>
         <v>-2.769017341040361E-4</v>
       </c>
-      <c r="K16" s="10">
-        <f>_xlfn.RANK.EQ($J16, $J$2:$J$52) +COUNTIF(J$2:J16,J16) -1</f>
-        <v>6</v>
+      <c r="K16" s="9">
+        <f>_xlfn.RANK.EQ($J16, $J$2:$J$52, 1) +COUNTIF(J$2:J16,J16) -1</f>
+        <v>46</v>
       </c>
       <c r="L16">
         <v>7397200</v>
@@ -2134,9 +2135,9 @@
         <f t="shared" si="5"/>
         <v>-1.4464932677229222E-5</v>
       </c>
-      <c r="P16" s="10">
-        <f>_xlfn.RANK.EQ($O16, $O$2:$O$52) +COUNTIF(O$2:O16,O16) -1</f>
-        <v>9</v>
+      <c r="P16" s="9">
+        <f>_xlfn.RANK.EQ($O16, $O$2:$O$52, 1) +COUNTIF(O$2:O16,O16) -1</f>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -2158,8 +2159,8 @@
         <v>-2.8351094826658003E-2</v>
       </c>
       <c r="F17" s="9">
-        <f>_xlfn.RANK.EQ($E17, $E$2:$E$52) +COUNTIF(E$2:E17,E17) -1</f>
-        <v>31</v>
+        <f>_xlfn.RANK.EQ($E17, $E$2:$E$52, 1) +COUNTIF(E$2:E17,E17) -1</f>
+        <v>21</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -2175,9 +2176,9 @@
         <f t="shared" si="3"/>
         <v>-4.3401666263871937E-2</v>
       </c>
-      <c r="K17" s="10">
-        <f>_xlfn.RANK.EQ($J17, $J$2:$J$52) +COUNTIF(J$2:J17,J17) -1</f>
-        <v>27</v>
+      <c r="K17" s="9">
+        <f>_xlfn.RANK.EQ($J17, $J$2:$J$52, 1) +COUNTIF(J$2:J17,J17) -1</f>
+        <v>25</v>
       </c>
       <c r="L17">
         <v>15311800</v>
@@ -2193,9 +2194,9 @@
         <f t="shared" si="5"/>
         <v>-6.3071811282801551E-2</v>
       </c>
-      <c r="P17" s="10">
-        <f>_xlfn.RANK.EQ($O17, $O$2:$O$52) +COUNTIF(O$2:O17,O17) -1</f>
-        <v>41</v>
+      <c r="P17" s="9">
+        <f>_xlfn.RANK.EQ($O17, $O$2:$O$52, 1) +COUNTIF(O$2:O17,O17) -1</f>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -2217,8 +2218,8 @@
         <v>-5.4037002206391245E-2</v>
       </c>
       <c r="F18" s="9">
-        <f>_xlfn.RANK.EQ($E18, $E$2:$E$52) +COUNTIF(E$2:E18,E18) -1</f>
-        <v>40</v>
+        <f>_xlfn.RANK.EQ($E18, $E$2:$E$52, 1) +COUNTIF(E$2:E18,E18) -1</f>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -2234,9 +2235,9 @@
         <f t="shared" si="3"/>
         <v>-6.6149619014330668E-2</v>
       </c>
-      <c r="K18" s="10">
-        <f>_xlfn.RANK.EQ($J18, $J$2:$J$52) +COUNTIF(J$2:J18,J18) -1</f>
-        <v>37</v>
+      <c r="K18" s="9">
+        <f>_xlfn.RANK.EQ($J18, $J$2:$J$52, 1) +COUNTIF(J$2:J18,J18) -1</f>
+        <v>15</v>
       </c>
       <c r="L18">
         <v>2910600</v>
@@ -2252,9 +2253,9 @@
         <f t="shared" si="5"/>
         <v>-0.12882667147667154</v>
       </c>
-      <c r="P18" s="10">
-        <f>_xlfn.RANK.EQ($O18, $O$2:$O$52) +COUNTIF(O$2:O18,O18) -1</f>
-        <v>49</v>
+      <c r="P18" s="9">
+        <f>_xlfn.RANK.EQ($O18, $O$2:$O$52, 1) +COUNTIF(O$2:O18,O18) -1</f>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -2276,8 +2277,8 @@
         <v>-4.258504294298146E-2</v>
       </c>
       <c r="F19" s="9">
-        <f>_xlfn.RANK.EQ($E19, $E$2:$E$52) +COUNTIF(E$2:E19,E19) -1</f>
-        <v>37</v>
+        <f>_xlfn.RANK.EQ($E19, $E$2:$E$52, 1) +COUNTIF(E$2:E19,E19) -1</f>
+        <v>15</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -2293,9 +2294,9 @@
         <f t="shared" si="3"/>
         <v>-7.4289145810384635E-2</v>
       </c>
-      <c r="K19" s="10">
-        <f>_xlfn.RANK.EQ($J19, $J$2:$J$52) +COUNTIF(J$2:J19,J19) -1</f>
-        <v>40</v>
+      <c r="K19" s="9">
+        <f>_xlfn.RANK.EQ($J19, $J$2:$J$52, 1) +COUNTIF(J$2:J19,J19) -1</f>
+        <v>12</v>
       </c>
       <c r="L19">
         <v>9343000</v>
@@ -2311,9 +2312,9 @@
         <f t="shared" si="5"/>
         <v>-6.1687262121374278E-2</v>
       </c>
-      <c r="P19" s="10">
-        <f>_xlfn.RANK.EQ($O19, $O$2:$O$52) +COUNTIF(O$2:O19,O19) -1</f>
-        <v>40</v>
+      <c r="P19" s="9">
+        <f>_xlfn.RANK.EQ($O19, $O$2:$O$52, 1) +COUNTIF(O$2:O19,O19) -1</f>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -2335,8 +2336,8 @@
         <v>-1.2379538203300809E-5</v>
       </c>
       <c r="F20" s="9">
-        <f>_xlfn.RANK.EQ($E20, $E$2:$E$52) +COUNTIF(E$2:E20,E20) -1</f>
-        <v>6</v>
+        <f>_xlfn.RANK.EQ($E20, $E$2:$E$52, 1) +COUNTIF(E$2:E20,E20) -1</f>
+        <v>46</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -2352,9 +2353,9 @@
         <f t="shared" si="3"/>
         <v>-7.4142392760188761E-5</v>
       </c>
-      <c r="K20" s="10">
-        <f>_xlfn.RANK.EQ($J20, $J$2:$J$52) +COUNTIF(J$2:J20,J20) -1</f>
-        <v>5</v>
+      <c r="K20" s="9">
+        <f>_xlfn.RANK.EQ($J20, $J$2:$J$52, 1) +COUNTIF(J$2:J20,J20) -1</f>
+        <v>47</v>
       </c>
       <c r="L20">
         <v>130621400</v>
@@ -2370,9 +2371,9 @@
         <f t="shared" si="5"/>
         <v>-8.9158438821450736E-7</v>
       </c>
-      <c r="P20" s="10">
-        <f>_xlfn.RANK.EQ($O20, $O$2:$O$52) +COUNTIF(O$2:O20,O20) -1</f>
-        <v>6</v>
+      <c r="P20" s="9">
+        <f>_xlfn.RANK.EQ($O20, $O$2:$O$52, 1) +COUNTIF(O$2:O20,O20) -1</f>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -2394,8 +2395,8 @@
         <v>-7.9052463618023094E-2</v>
       </c>
       <c r="F21" s="9">
-        <f>_xlfn.RANK.EQ($E21, $E$2:$E$52) +COUNTIF(E$2:E21,E21) -1</f>
-        <v>43</v>
+        <f>_xlfn.RANK.EQ($E21, $E$2:$E$52, 1) +COUNTIF(E$2:E21,E21) -1</f>
+        <v>9</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -2411,9 +2412,9 @@
         <f t="shared" si="3"/>
         <v>-7.5167420624229556E-2</v>
       </c>
-      <c r="K21" s="10">
-        <f>_xlfn.RANK.EQ($J21, $J$2:$J$52) +COUNTIF(J$2:J21,J21) -1</f>
-        <v>41</v>
+      <c r="K21" s="9">
+        <f>_xlfn.RANK.EQ($J21, $J$2:$J$52, 1) +COUNTIF(J$2:J21,J21) -1</f>
+        <v>11</v>
       </c>
       <c r="L21">
         <v>24323000</v>
@@ -2429,9 +2430,9 @@
         <f t="shared" si="5"/>
         <v>-3.6546762734864152E-2</v>
       </c>
-      <c r="P21" s="10">
-        <f>_xlfn.RANK.EQ($O21, $O$2:$O$52) +COUNTIF(O$2:O21,O21) -1</f>
-        <v>31</v>
+      <c r="P21" s="9">
+        <f>_xlfn.RANK.EQ($O21, $O$2:$O$52, 1) +COUNTIF(O$2:O21,O21) -1</f>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2453,8 +2454,8 @@
         <v>-1.3285502334437123E-2</v>
       </c>
       <c r="F22" s="9">
-        <f>_xlfn.RANK.EQ($E22, $E$2:$E$52) +COUNTIF(E$2:E22,E22) -1</f>
-        <v>20</v>
+        <f>_xlfn.RANK.EQ($E22, $E$2:$E$52, 1) +COUNTIF(E$2:E22,E22) -1</f>
+        <v>32</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -2470,9 +2471,9 @@
         <f t="shared" si="3"/>
         <v>-1.5752170574348738E-2</v>
       </c>
-      <c r="K22" s="10">
-        <f>_xlfn.RANK.EQ($J22, $J$2:$J$52) +COUNTIF(J$2:J22,J22) -1</f>
-        <v>14</v>
+      <c r="K22" s="9">
+        <f>_xlfn.RANK.EQ($J22, $J$2:$J$52, 1) +COUNTIF(J$2:J22,J22) -1</f>
+        <v>38</v>
       </c>
       <c r="L22">
         <v>11935200</v>
@@ -2488,9 +2489,9 @@
         <f t="shared" si="5"/>
         <v>-6.2439674240938325E-5</v>
       </c>
-      <c r="P22" s="10">
-        <f>_xlfn.RANK.EQ($O22, $O$2:$O$52) +COUNTIF(O$2:O22,O22) -1</f>
-        <v>10</v>
+      <c r="P22" s="9">
+        <f>_xlfn.RANK.EQ($O22, $O$2:$O$52, 1) +COUNTIF(O$2:O22,O22) -1</f>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2512,8 +2513,8 @@
         <v>-3.9590110100806722E-2</v>
       </c>
       <c r="F23" s="9">
-        <f>_xlfn.RANK.EQ($E23, $E$2:$E$52) +COUNTIF(E$2:E23,E23) -1</f>
-        <v>34</v>
+        <f>_xlfn.RANK.EQ($E23, $E$2:$E$52, 1) +COUNTIF(E$2:E23,E23) -1</f>
+        <v>18</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -2529,8 +2530,8 @@
         <f t="shared" si="3"/>
         <v>-4.2394738976719144E-2</v>
       </c>
-      <c r="K23" s="10">
-        <f>_xlfn.RANK.EQ($J23, $J$2:$J$52) +COUNTIF(J$2:J23,J23) -1</f>
+      <c r="K23" s="9">
+        <f>_xlfn.RANK.EQ($J23, $J$2:$J$52, 1) +COUNTIF(J$2:J23,J23) -1</f>
         <v>26</v>
       </c>
       <c r="L23">
@@ -2547,8 +2548,8 @@
         <f t="shared" si="5"/>
         <v>-2.5892971236375011E-2</v>
       </c>
-      <c r="P23" s="10">
-        <f>_xlfn.RANK.EQ($O23, $O$2:$O$52) +COUNTIF(O$2:O23,O23) -1</f>
+      <c r="P23" s="9">
+        <f>_xlfn.RANK.EQ($O23, $O$2:$O$52, 1) +COUNTIF(O$2:O23,O23) -1</f>
         <v>26</v>
       </c>
     </row>
@@ -2571,8 +2572,8 @@
         <v>-1.3334943305713101E-2</v>
       </c>
       <c r="F24" s="9">
-        <f>_xlfn.RANK.EQ($E24, $E$2:$E$52) +COUNTIF(E$2:E24,E24) -1</f>
-        <v>21</v>
+        <f>_xlfn.RANK.EQ($E24, $E$2:$E$52, 1) +COUNTIF(E$2:E24,E24) -1</f>
+        <v>31</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -2588,9 +2589,9 @@
         <f t="shared" si="3"/>
         <v>-4.087856565111897E-2</v>
       </c>
-      <c r="K24" s="10">
-        <f>_xlfn.RANK.EQ($J24, $J$2:$J$52) +COUNTIF(J$2:J24,J24) -1</f>
-        <v>24</v>
+      <c r="K24" s="9">
+        <f>_xlfn.RANK.EQ($J24, $J$2:$J$52, 1) +COUNTIF(J$2:J24,J24) -1</f>
+        <v>28</v>
       </c>
       <c r="L24">
         <v>1112600</v>
@@ -2606,9 +2607,9 @@
         <f t="shared" si="5"/>
         <v>-6.5504224339284781E-5</v>
       </c>
-      <c r="P24" s="10">
-        <f>_xlfn.RANK.EQ($O24, $O$2:$O$52) +COUNTIF(O$2:O24,O24) -1</f>
-        <v>11</v>
+      <c r="P24" s="9">
+        <f>_xlfn.RANK.EQ($O24, $O$2:$O$52, 1) +COUNTIF(O$2:O24,O24) -1</f>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -2630,8 +2631,8 @@
         <v>-1.0226130964676661E-2</v>
       </c>
       <c r="F25" s="9">
-        <f>_xlfn.RANK.EQ($E25, $E$2:$E$52) +COUNTIF(E$2:E25,E25) -1</f>
-        <v>14</v>
+        <f>_xlfn.RANK.EQ($E25, $E$2:$E$52, 1) +COUNTIF(E$2:E25,E25) -1</f>
+        <v>38</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -2647,9 +2648,9 @@
         <f t="shared" si="3"/>
         <v>-1.5846773555029746E-2</v>
       </c>
-      <c r="K25" s="10">
-        <f>_xlfn.RANK.EQ($J25, $J$2:$J$52) +COUNTIF(J$2:J25,J25) -1</f>
-        <v>15</v>
+      <c r="K25" s="9">
+        <f>_xlfn.RANK.EQ($J25, $J$2:$J$52, 1) +COUNTIF(J$2:J25,J25) -1</f>
+        <v>37</v>
       </c>
       <c r="L25">
         <v>496500</v>
@@ -2665,9 +2666,9 @@
         <f t="shared" si="5"/>
         <v>-3.4741188318228064E-3</v>
       </c>
-      <c r="P25" s="10">
-        <f>_xlfn.RANK.EQ($O25, $O$2:$O$52) +COUNTIF(O$2:O25,O25) -1</f>
-        <v>17</v>
+      <c r="P25" s="9">
+        <f>_xlfn.RANK.EQ($O25, $O$2:$O$52, 1) +COUNTIF(O$2:O25,O25) -1</f>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -2689,8 +2690,8 @@
         <v>-8.5306091660634673E-2</v>
       </c>
       <c r="F26" s="9">
-        <f>_xlfn.RANK.EQ($E26, $E$2:$E$52) +COUNTIF(E$2:E26,E26) -1</f>
-        <v>47</v>
+        <f>_xlfn.RANK.EQ($E26, $E$2:$E$52, 1) +COUNTIF(E$2:E26,E26) -1</f>
+        <v>5</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -2706,9 +2707,9 @@
         <f t="shared" si="3"/>
         <v>-5.8776040939327839E-2</v>
       </c>
-      <c r="K26" s="10">
-        <f>_xlfn.RANK.EQ($J26, $J$2:$J$52) +COUNTIF(J$2:J26,J26) -1</f>
-        <v>36</v>
+      <c r="K26" s="9">
+        <f>_xlfn.RANK.EQ($J26, $J$2:$J$52, 1) +COUNTIF(J$2:J26,J26) -1</f>
+        <v>16</v>
       </c>
       <c r="L26">
         <v>5430700</v>
@@ -2724,9 +2725,9 @@
         <f t="shared" si="5"/>
         <v>-5.7720881286022069E-2</v>
       </c>
-      <c r="P26" s="10">
-        <f>_xlfn.RANK.EQ($O26, $O$2:$O$52) +COUNTIF(O$2:O26,O26) -1</f>
-        <v>39</v>
+      <c r="P26" s="9">
+        <f>_xlfn.RANK.EQ($O26, $O$2:$O$52, 1) +COUNTIF(O$2:O26,O26) -1</f>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -2748,8 +2749,8 @@
         <v>0</v>
       </c>
       <c r="F27" s="9">
-        <f>_xlfn.RANK.EQ($E27, $E$2:$E$52) +COUNTIF(E$2:E27,E27) -1</f>
-        <v>3</v>
+        <f>_xlfn.RANK.EQ($E27, $E$2:$E$52, 1) +COUNTIF(E$2:E27,E27) -1</f>
+        <v>48</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -2765,9 +2766,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K27" s="10">
-        <f>_xlfn.RANK.EQ($J27, $J$2:$J$52) +COUNTIF(J$2:J27,J27) -1</f>
-        <v>2</v>
+      <c r="K27" s="9">
+        <f>_xlfn.RANK.EQ($J27, $J$2:$J$52, 1) +COUNTIF(J$2:J27,J27) -1</f>
+        <v>49</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -2783,9 +2784,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P27" s="10">
-        <f>_xlfn.RANK.EQ($O27, $O$2:$O$52) +COUNTIF(O$2:O27,O27) -1</f>
-        <v>1</v>
+      <c r="P27" s="9">
+        <f>_xlfn.RANK.EQ($O27, $O$2:$O$52, 1) +COUNTIF(O$2:O27,O27) -1</f>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -2807,8 +2808,8 @@
         <v>-9.5782760864849215E-2</v>
       </c>
       <c r="F28" s="9">
-        <f>_xlfn.RANK.EQ($E28, $E$2:$E$52) +COUNTIF(E$2:E28,E28) -1</f>
-        <v>49</v>
+        <f>_xlfn.RANK.EQ($E28, $E$2:$E$52, 1) +COUNTIF(E$2:E28,E28) -1</f>
+        <v>3</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -2824,9 +2825,9 @@
         <f t="shared" si="3"/>
         <v>-0.17103239309050916</v>
       </c>
-      <c r="K28" s="10">
-        <f>_xlfn.RANK.EQ($J28, $J$2:$J$52) +COUNTIF(J$2:J28,J28) -1</f>
-        <v>50</v>
+      <c r="K28" s="9">
+        <f>_xlfn.RANK.EQ($J28, $J$2:$J$52, 1) +COUNTIF(J$2:J28,J28) -1</f>
+        <v>2</v>
       </c>
       <c r="L28">
         <v>1525900</v>
@@ -2842,9 +2843,9 @@
         <f t="shared" si="5"/>
         <v>-8.6909325643882263E-2</v>
       </c>
-      <c r="P28" s="10">
-        <f>_xlfn.RANK.EQ($O28, $O$2:$O$52) +COUNTIF(O$2:O28,O28) -1</f>
-        <v>45</v>
+      <c r="P28" s="9">
+        <f>_xlfn.RANK.EQ($O28, $O$2:$O$52, 1) +COUNTIF(O$2:O28,O28) -1</f>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -2866,8 +2867,8 @@
         <v>-1.4800253727847622E-2</v>
       </c>
       <c r="F29" s="9">
-        <f>_xlfn.RANK.EQ($E29, $E$2:$E$52) +COUNTIF(E$2:E29,E29) -1</f>
-        <v>24</v>
+        <f>_xlfn.RANK.EQ($E29, $E$2:$E$52, 1) +COUNTIF(E$2:E29,E29) -1</f>
+        <v>28</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -2883,9 +2884,9 @@
         <f t="shared" si="3"/>
         <v>-4.1099320021590155E-2</v>
       </c>
-      <c r="K29" s="10">
-        <f>_xlfn.RANK.EQ($J29, $J$2:$J$52) +COUNTIF(J$2:J29,J29) -1</f>
-        <v>25</v>
+      <c r="K29" s="9">
+        <f>_xlfn.RANK.EQ($J29, $J$2:$J$52, 1) +COUNTIF(J$2:J29,J29) -1</f>
+        <v>27</v>
       </c>
       <c r="L29">
         <v>2889900</v>
@@ -2901,9 +2902,9 @@
         <f t="shared" si="5"/>
         <v>-1.2225336516860273E-5</v>
       </c>
-      <c r="P29" s="10">
-        <f>_xlfn.RANK.EQ($O29, $O$2:$O$52) +COUNTIF(O$2:O29,O29) -1</f>
-        <v>8</v>
+      <c r="P29" s="9">
+        <f>_xlfn.RANK.EQ($O29, $O$2:$O$52, 1) +COUNTIF(O$2:O29,O29) -1</f>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -2925,8 +2926,8 @@
         <v>-8.3831374359143746E-3</v>
       </c>
       <c r="F30" s="9">
-        <f>_xlfn.RANK.EQ($E30, $E$2:$E$52) +COUNTIF(E$2:E30,E30) -1</f>
-        <v>12</v>
+        <f>_xlfn.RANK.EQ($E30, $E$2:$E$52, 1) +COUNTIF(E$2:E30,E30) -1</f>
+        <v>40</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -2942,9 +2943,9 @@
         <f t="shared" si="3"/>
         <v>-3.9561962641116366E-3</v>
       </c>
-      <c r="K30" s="10">
-        <f>_xlfn.RANK.EQ($J30, $J$2:$J$52) +COUNTIF(J$2:J30,J30) -1</f>
-        <v>10</v>
+      <c r="K30" s="9">
+        <f>_xlfn.RANK.EQ($J30, $J$2:$J$52, 1) +COUNTIF(J$2:J30,J30) -1</f>
+        <v>42</v>
       </c>
       <c r="L30">
         <v>12861300</v>
@@ -2960,9 +2961,9 @@
         <f t="shared" si="5"/>
         <v>-2.7439209100169185E-3</v>
       </c>
-      <c r="P30" s="10">
-        <f>_xlfn.RANK.EQ($O30, $O$2:$O$52) +COUNTIF(O$2:O30,O30) -1</f>
-        <v>16</v>
+      <c r="P30" s="9">
+        <f>_xlfn.RANK.EQ($O30, $O$2:$O$52, 1) +COUNTIF(O$2:O30,O30) -1</f>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2984,8 +2985,8 @@
         <v>-1.4030533529678329E-2</v>
       </c>
       <c r="F31" s="9">
-        <f>_xlfn.RANK.EQ($E31, $E$2:$E$52) +COUNTIF(E$2:E31,E31) -1</f>
-        <v>23</v>
+        <f>_xlfn.RANK.EQ($E31, $E$2:$E$52, 1) +COUNTIF(E$2:E31,E31) -1</f>
+        <v>29</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -3001,9 +3002,9 @@
         <f t="shared" si="3"/>
         <v>-3.3249136181648611E-2</v>
       </c>
-      <c r="K31" s="10">
-        <f>_xlfn.RANK.EQ($J31, $J$2:$J$52) +COUNTIF(J$2:J31,J31) -1</f>
-        <v>20</v>
+      <c r="K31" s="9">
+        <f>_xlfn.RANK.EQ($J31, $J$2:$J$52, 1) +COUNTIF(J$2:J31,J31) -1</f>
+        <v>32</v>
       </c>
       <c r="L31">
         <v>1870700</v>
@@ -3019,9 +3020,9 @@
         <f t="shared" si="5"/>
         <v>-3.7049585716576634E-2</v>
       </c>
-      <c r="P31" s="10">
-        <f>_xlfn.RANK.EQ($O31, $O$2:$O$52) +COUNTIF(O$2:O31,O31) -1</f>
-        <v>32</v>
+      <c r="P31" s="9">
+        <f>_xlfn.RANK.EQ($O31, $O$2:$O$52, 1) +COUNTIF(O$2:O31,O31) -1</f>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -3043,8 +3044,8 @@
         <v>-1.2294942827617691E-2</v>
       </c>
       <c r="F32" s="9">
-        <f>_xlfn.RANK.EQ($E32, $E$2:$E$52) +COUNTIF(E$2:E32,E32) -1</f>
-        <v>16</v>
+        <f>_xlfn.RANK.EQ($E32, $E$2:$E$52, 1) +COUNTIF(E$2:E32,E32) -1</f>
+        <v>36</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -3060,9 +3061,9 @@
         <f t="shared" si="3"/>
         <v>-1.7837871035428981E-2</v>
       </c>
-      <c r="K32" s="10">
-        <f>_xlfn.RANK.EQ($J32, $J$2:$J$52) +COUNTIF(J$2:J32,J32) -1</f>
-        <v>17</v>
+      <c r="K32" s="9">
+        <f>_xlfn.RANK.EQ($J32, $J$2:$J$52, 1) +COUNTIF(J$2:J32,J32) -1</f>
+        <v>35</v>
       </c>
       <c r="L32">
         <v>6157400</v>
@@ -3078,9 +3079,9 @@
         <f t="shared" si="5"/>
         <v>-2.7581118653977402E-2</v>
       </c>
-      <c r="P32" s="10">
-        <f>_xlfn.RANK.EQ($O32, $O$2:$O$52) +COUNTIF(O$2:O32,O32) -1</f>
-        <v>29</v>
+      <c r="P32" s="9">
+        <f>_xlfn.RANK.EQ($O32, $O$2:$O$52, 1) +COUNTIF(O$2:O32,O32) -1</f>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -3102,8 +3103,8 @@
         <v>-7.9969930789269058E-3</v>
       </c>
       <c r="F33" s="9">
-        <f>_xlfn.RANK.EQ($E33, $E$2:$E$52) +COUNTIF(E$2:E33,E33) -1</f>
-        <v>11</v>
+        <f>_xlfn.RANK.EQ($E33, $E$2:$E$52, 1) +COUNTIF(E$2:E33,E33) -1</f>
+        <v>41</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -3119,9 +3120,9 @@
         <f t="shared" si="3"/>
         <v>-2.6564903115433454E-3</v>
       </c>
-      <c r="K33" s="10">
-        <f>_xlfn.RANK.EQ($J33, $J$2:$J$52) +COUNTIF(J$2:J33,J33) -1</f>
-        <v>9</v>
+      <c r="K33" s="9">
+        <f>_xlfn.RANK.EQ($J33, $J$2:$J$52, 1) +COUNTIF(J$2:J33,J33) -1</f>
+        <v>43</v>
       </c>
       <c r="L33">
         <v>989572899.99999905</v>
@@ -3137,9 +3138,9 @@
         <f t="shared" si="5"/>
         <v>-5.5141067323084929E-3</v>
       </c>
-      <c r="P33" s="10">
-        <f>_xlfn.RANK.EQ($O33, $O$2:$O$52) +COUNTIF(O$2:O33,O33) -1</f>
-        <v>18</v>
+      <c r="P33" s="9">
+        <f>_xlfn.RANK.EQ($O33, $O$2:$O$52, 1) +COUNTIF(O$2:O33,O33) -1</f>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -3161,7 +3162,7 @@
         <v>-1.8939149738619768E-2</v>
       </c>
       <c r="F34" s="9">
-        <f>_xlfn.RANK.EQ($E34, $E$2:$E$52) +COUNTIF(E$2:E34,E34) -1</f>
+        <f>_xlfn.RANK.EQ($E34, $E$2:$E$52, 1) +COUNTIF(E$2:E34,E34) -1</f>
         <v>26</v>
       </c>
       <c r="G34">
@@ -3178,9 +3179,9 @@
         <f t="shared" si="3"/>
         <v>-4.8961345561534093E-2</v>
       </c>
-      <c r="K34" s="10">
-        <f>_xlfn.RANK.EQ($J34, $J$2:$J$52) +COUNTIF(J$2:J34,J34) -1</f>
-        <v>31</v>
+      <c r="K34" s="9">
+        <f>_xlfn.RANK.EQ($J34, $J$2:$J$52, 1) +COUNTIF(J$2:J34,J34) -1</f>
+        <v>21</v>
       </c>
       <c r="L34">
         <v>4345600</v>
@@ -3196,9 +3197,9 @@
         <f t="shared" si="5"/>
         <v>-2.6647296115611244E-2</v>
       </c>
-      <c r="P34" s="10">
-        <f>_xlfn.RANK.EQ($O34, $O$2:$O$52) +COUNTIF(O$2:O34,O34) -1</f>
-        <v>28</v>
+      <c r="P34" s="9">
+        <f>_xlfn.RANK.EQ($O34, $O$2:$O$52, 1) +COUNTIF(O$2:O34,O34) -1</f>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -3220,8 +3221,8 @@
         <v>0</v>
       </c>
       <c r="F35" s="9">
-        <f>_xlfn.RANK.EQ($E35, $E$2:$E$52) +COUNTIF(E$2:E35,E35) -1</f>
-        <v>4</v>
+        <f>_xlfn.RANK.EQ($E35, $E$2:$E$52, 1) +COUNTIF(E$2:E35,E35) -1</f>
+        <v>49</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -3237,9 +3238,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K35" s="10">
-        <f>_xlfn.RANK.EQ($J35, $J$2:$J$52) +COUNTIF(J$2:J35,J35) -1</f>
-        <v>3</v>
+      <c r="K35" s="9">
+        <f>_xlfn.RANK.EQ($J35, $J$2:$J$52, 1) +COUNTIF(J$2:J35,J35) -1</f>
+        <v>50</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -3255,9 +3256,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P35" s="10">
-        <f>_xlfn.RANK.EQ($O35, $O$2:$O$52) +COUNTIF(O$2:O35,O35) -1</f>
-        <v>2</v>
+      <c r="P35" s="9">
+        <f>_xlfn.RANK.EQ($O35, $O$2:$O$52, 1) +COUNTIF(O$2:O35,O35) -1</f>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -3279,8 +3280,8 @@
         <v>-7.8647857679780775E-2</v>
       </c>
       <c r="F36" s="9">
-        <f>_xlfn.RANK.EQ($E36, $E$2:$E$52) +COUNTIF(E$2:E36,E36) -1</f>
-        <v>42</v>
+        <f>_xlfn.RANK.EQ($E36, $E$2:$E$52, 1) +COUNTIF(E$2:E36,E36) -1</f>
+        <v>10</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -3296,9 +3297,9 @@
         <f t="shared" si="3"/>
         <v>-0.17551246244575608</v>
       </c>
-      <c r="K36" s="10">
-        <f>_xlfn.RANK.EQ($J36, $J$2:$J$52) +COUNTIF(J$2:J36,J36) -1</f>
-        <v>51</v>
+      <c r="K36" s="9">
+        <f>_xlfn.RANK.EQ($J36, $J$2:$J$52, 1) +COUNTIF(J$2:J36,J36) -1</f>
+        <v>1</v>
       </c>
       <c r="L36">
         <v>878300</v>
@@ -3314,9 +3315,9 @@
         <f t="shared" si="5"/>
         <v>-0.11509132414892521</v>
       </c>
-      <c r="P36" s="10">
-        <f>_xlfn.RANK.EQ($O36, $O$2:$O$52) +COUNTIF(O$2:O36,O36) -1</f>
-        <v>47</v>
+      <c r="P36" s="9">
+        <f>_xlfn.RANK.EQ($O36, $O$2:$O$52, 1) +COUNTIF(O$2:O36,O36) -1</f>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -3338,8 +3339,8 @@
         <v>-3.9444515758219188E-2</v>
       </c>
       <c r="F37" s="9">
-        <f>_xlfn.RANK.EQ($E37, $E$2:$E$52) +COUNTIF(E$2:E37,E37) -1</f>
-        <v>33</v>
+        <f>_xlfn.RANK.EQ($E37, $E$2:$E$52, 1) +COUNTIF(E$2:E37,E37) -1</f>
+        <v>19</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -3355,9 +3356,9 @@
         <f t="shared" si="3"/>
         <v>-4.9460250314014013E-2</v>
       </c>
-      <c r="K37" s="10">
-        <f>_xlfn.RANK.EQ($J37, $J$2:$J$52) +COUNTIF(J$2:J37,J37) -1</f>
-        <v>32</v>
+      <c r="K37" s="9">
+        <f>_xlfn.RANK.EQ($J37, $J$2:$J$52, 1) +COUNTIF(J$2:J37,J37) -1</f>
+        <v>20</v>
       </c>
       <c r="L37">
         <v>2296900</v>
@@ -3373,9 +3374,9 @@
         <f t="shared" si="5"/>
         <v>-8.1928538464887526E-2</v>
       </c>
-      <c r="P37" s="10">
-        <f>_xlfn.RANK.EQ($O37, $O$2:$O$52) +COUNTIF(O$2:O37,O37) -1</f>
-        <v>44</v>
+      <c r="P37" s="9">
+        <f>_xlfn.RANK.EQ($O37, $O$2:$O$52, 1) +COUNTIF(O$2:O37,O37) -1</f>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -3397,8 +3398,8 @@
         <v>-1.9443680579913542E-2</v>
       </c>
       <c r="F38" s="9">
-        <f>_xlfn.RANK.EQ($E38, $E$2:$E$52) +COUNTIF(E$2:E38,E38) -1</f>
-        <v>27</v>
+        <f>_xlfn.RANK.EQ($E38, $E$2:$E$52, 1) +COUNTIF(E$2:E38,E38) -1</f>
+        <v>25</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -3414,9 +3415,9 @@
         <f t="shared" si="3"/>
         <v>-4.9631735620585316E-2</v>
       </c>
-      <c r="K38" s="10">
-        <f>_xlfn.RANK.EQ($J38, $J$2:$J$52) +COUNTIF(J$2:J38,J38) -1</f>
-        <v>33</v>
+      <c r="K38" s="9">
+        <f>_xlfn.RANK.EQ($J38, $J$2:$J$52, 1) +COUNTIF(J$2:J38,J38) -1</f>
+        <v>19</v>
       </c>
       <c r="L38">
         <v>777800</v>
@@ -3432,9 +3433,9 @@
         <f t="shared" si="5"/>
         <v>-1.7580354847003174E-4</v>
       </c>
-      <c r="P38" s="10">
-        <f>_xlfn.RANK.EQ($O38, $O$2:$O$52) +COUNTIF(O$2:O38,O38) -1</f>
-        <v>12</v>
+      <c r="P38" s="9">
+        <f>_xlfn.RANK.EQ($O38, $O$2:$O$52, 1) +COUNTIF(O$2:O38,O38) -1</f>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -3456,8 +3457,8 @@
         <v>-8.008952370177623E-2</v>
       </c>
       <c r="F39" s="9">
-        <f>_xlfn.RANK.EQ($E39, $E$2:$E$52) +COUNTIF(E$2:E39,E39) -1</f>
-        <v>44</v>
+        <f>_xlfn.RANK.EQ($E39, $E$2:$E$52, 1) +COUNTIF(E$2:E39,E39) -1</f>
+        <v>8</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -3473,9 +3474,9 @@
         <f t="shared" si="3"/>
         <v>-0.13918241656366656</v>
       </c>
-      <c r="K39" s="10">
-        <f>_xlfn.RANK.EQ($J39, $J$2:$J$52) +COUNTIF(J$2:J39,J39) -1</f>
-        <v>49</v>
+      <c r="K39" s="9">
+        <f>_xlfn.RANK.EQ($J39, $J$2:$J$52, 1) +COUNTIF(J$2:J39,J39) -1</f>
+        <v>3</v>
       </c>
       <c r="L39">
         <v>1759500</v>
@@ -3491,9 +3492,9 @@
         <f t="shared" si="5"/>
         <v>-4.4919653310605226E-2</v>
       </c>
-      <c r="P39" s="10">
-        <f>_xlfn.RANK.EQ($O39, $O$2:$O$52) +COUNTIF(O$2:O39,O39) -1</f>
-        <v>35</v>
+      <c r="P39" s="9">
+        <f>_xlfn.RANK.EQ($O39, $O$2:$O$52, 1) +COUNTIF(O$2:O39,O39) -1</f>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -3515,8 +3516,8 @@
         <v>-2.1279773539092578E-2</v>
       </c>
       <c r="F40" s="9">
-        <f>_xlfn.RANK.EQ($E40, $E$2:$E$52) +COUNTIF(E$2:E40,E40) -1</f>
-        <v>29</v>
+        <f>_xlfn.RANK.EQ($E40, $E$2:$E$52, 1) +COUNTIF(E$2:E40,E40) -1</f>
+        <v>23</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -3532,9 +3533,9 @@
         <f t="shared" si="3"/>
         <v>-4.6782546934937892E-2</v>
       </c>
-      <c r="K40" s="10">
-        <f>_xlfn.RANK.EQ($J40, $J$2:$J$52) +COUNTIF(J$2:J40,J40) -1</f>
-        <v>30</v>
+      <c r="K40" s="9">
+        <f>_xlfn.RANK.EQ($J40, $J$2:$J$52, 1) +COUNTIF(J$2:J40,J40) -1</f>
+        <v>22</v>
       </c>
       <c r="L40">
         <v>40216700</v>
@@ -3550,9 +3551,9 @@
         <f t="shared" si="5"/>
         <v>-1.5178676768608648E-2</v>
       </c>
-      <c r="P40" s="10">
-        <f>_xlfn.RANK.EQ($O40, $O$2:$O$52) +COUNTIF(O$2:O40,O40) -1</f>
-        <v>21</v>
+      <c r="P40" s="9">
+        <f>_xlfn.RANK.EQ($O40, $O$2:$O$52, 1) +COUNTIF(O$2:O40,O40) -1</f>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -3574,8 +3575,8 @@
         <v>-4.0110550149132493E-2</v>
       </c>
       <c r="F41" s="9">
-        <f>_xlfn.RANK.EQ($E41, $E$2:$E$52) +COUNTIF(E$2:E41,E41) -1</f>
-        <v>35</v>
+        <f>_xlfn.RANK.EQ($E41, $E$2:$E$52, 1) +COUNTIF(E$2:E41,E41) -1</f>
+        <v>17</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -3591,9 +3592,9 @@
         <f t="shared" si="3"/>
         <v>-2.6221894095689226E-2</v>
       </c>
-      <c r="K41" s="10">
-        <f>_xlfn.RANK.EQ($J41, $J$2:$J$52) +COUNTIF(J$2:J41,J41) -1</f>
-        <v>18</v>
+      <c r="K41" s="9">
+        <f>_xlfn.RANK.EQ($J41, $J$2:$J$52, 1) +COUNTIF(J$2:J41,J41) -1</f>
+        <v>34</v>
       </c>
       <c r="L41">
         <v>4799900</v>
@@ -3609,9 +3610,9 @@
         <f t="shared" si="5"/>
         <v>-1.7099804162586642E-2</v>
       </c>
-      <c r="P41" s="10">
-        <f>_xlfn.RANK.EQ($O41, $O$2:$O$52) +COUNTIF(O$2:O41,O41) -1</f>
-        <v>22</v>
+      <c r="P41" s="9">
+        <f>_xlfn.RANK.EQ($O41, $O$2:$O$52, 1) +COUNTIF(O$2:O41,O41) -1</f>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -3633,8 +3634,8 @@
         <v>-2.2070943135841053E-4</v>
       </c>
       <c r="F42" s="9">
-        <f>_xlfn.RANK.EQ($E42, $E$2:$E$52) +COUNTIF(E$2:E42,E42) -1</f>
-        <v>8</v>
+        <f>_xlfn.RANK.EQ($E42, $E$2:$E$52, 1) +COUNTIF(E$2:E42,E42) -1</f>
+        <v>44</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -3650,9 +3651,9 @@
         <f t="shared" si="3"/>
         <v>-1.1928203241796942E-2</v>
       </c>
-      <c r="K42" s="10">
-        <f>_xlfn.RANK.EQ($J42, $J$2:$J$52) +COUNTIF(J$2:J42,J42) -1</f>
-        <v>13</v>
+      <c r="K42" s="9">
+        <f>_xlfn.RANK.EQ($J42, $J$2:$J$52, 1) +COUNTIF(J$2:J42,J42) -1</f>
+        <v>39</v>
       </c>
       <c r="L42">
         <v>199954600</v>
@@ -3668,9 +3669,9 @@
         <f t="shared" si="5"/>
         <v>-1.8129115815929696E-7</v>
       </c>
-      <c r="P42" s="10">
-        <f>_xlfn.RANK.EQ($O42, $O$2:$O$52) +COUNTIF(O$2:O42,O42) -1</f>
-        <v>5</v>
+      <c r="P42" s="9">
+        <f>_xlfn.RANK.EQ($O42, $O$2:$O$52, 1) +COUNTIF(O$2:O42,O42) -1</f>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -3692,8 +3693,8 @@
         <v>-2.0497353541313264E-2</v>
       </c>
       <c r="F43" s="9">
-        <f>_xlfn.RANK.EQ($E43, $E$2:$E$52) +COUNTIF(E$2:E43,E43) -1</f>
-        <v>28</v>
+        <f>_xlfn.RANK.EQ($E43, $E$2:$E$52, 1) +COUNTIF(E$2:E43,E43) -1</f>
+        <v>24</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -3709,9 +3710,9 @@
         <f t="shared" si="3"/>
         <v>-4.5477990374731388E-2</v>
       </c>
-      <c r="K43" s="10">
-        <f>_xlfn.RANK.EQ($J43, $J$2:$J$52) +COUNTIF(J$2:J43,J43) -1</f>
-        <v>29</v>
+      <c r="K43" s="9">
+        <f>_xlfn.RANK.EQ($J43, $J$2:$J$52, 1) +COUNTIF(J$2:J43,J43) -1</f>
+        <v>23</v>
       </c>
       <c r="L43">
         <v>8497500</v>
@@ -3727,9 +3728,9 @@
         <f t="shared" si="5"/>
         <v>-4.0778750220654303E-2</v>
       </c>
-      <c r="P43" s="10">
-        <f>_xlfn.RANK.EQ($O43, $O$2:$O$52) +COUNTIF(O$2:O43,O43) -1</f>
-        <v>34</v>
+      <c r="P43" s="9">
+        <f>_xlfn.RANK.EQ($O43, $O$2:$O$52, 1) +COUNTIF(O$2:O43,O43) -1</f>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -3751,8 +3752,8 @@
         <v>-9.7760750186150751E-3</v>
       </c>
       <c r="F44" s="9">
-        <f>_xlfn.RANK.EQ($E44, $E$2:$E$52) +COUNTIF(E$2:E44,E44) -1</f>
-        <v>13</v>
+        <f>_xlfn.RANK.EQ($E44, $E$2:$E$52, 1) +COUNTIF(E$2:E44,E44) -1</f>
+        <v>39</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -3768,9 +3769,9 @@
         <f t="shared" si="3"/>
         <v>-7.9569249404813532E-3</v>
       </c>
-      <c r="K44" s="10">
-        <f>_xlfn.RANK.EQ($J44, $J$2:$J$52) +COUNTIF(J$2:J44,J44) -1</f>
-        <v>11</v>
+      <c r="K44" s="9">
+        <f>_xlfn.RANK.EQ($J44, $J$2:$J$52, 1) +COUNTIF(J$2:J44,J44) -1</f>
+        <v>41</v>
       </c>
       <c r="L44">
         <v>31282200</v>
@@ -3786,9 +3787,9 @@
         <f t="shared" si="5"/>
         <v>-1.8780648419868168E-6</v>
       </c>
-      <c r="P44" s="10">
-        <f>_xlfn.RANK.EQ($O44, $O$2:$O$52) +COUNTIF(O$2:O44,O44) -1</f>
-        <v>7</v>
+      <c r="P44" s="9">
+        <f>_xlfn.RANK.EQ($O44, $O$2:$O$52, 1) +COUNTIF(O$2:O44,O44) -1</f>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -3810,8 +3811,8 @@
         <v>-1.287514194887851E-2</v>
       </c>
       <c r="F45" s="9">
-        <f>_xlfn.RANK.EQ($E45, $E$2:$E$52) +COUNTIF(E$2:E45,E45) -1</f>
-        <v>18</v>
+        <f>_xlfn.RANK.EQ($E45, $E$2:$E$52, 1) +COUNTIF(E$2:E45,E45) -1</f>
+        <v>34</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -3827,9 +3828,9 @@
         <f t="shared" si="3"/>
         <v>-3.8689222111488959E-2</v>
       </c>
-      <c r="K45" s="10">
-        <f>_xlfn.RANK.EQ($J45, $J$2:$J$52) +COUNTIF(J$2:J45,J45) -1</f>
-        <v>22</v>
+      <c r="K45" s="9">
+        <f>_xlfn.RANK.EQ($J45, $J$2:$J$52, 1) +COUNTIF(J$2:J45,J45) -1</f>
+        <v>30</v>
       </c>
       <c r="L45">
         <v>56027100</v>
@@ -3845,9 +3846,9 @@
         <f t="shared" si="5"/>
         <v>-1.1432866237947358E-2</v>
       </c>
-      <c r="P45" s="10">
-        <f>_xlfn.RANK.EQ($O45, $O$2:$O$52) +COUNTIF(O$2:O45,O45) -1</f>
-        <v>20</v>
+      <c r="P45" s="9">
+        <f>_xlfn.RANK.EQ($O45, $O$2:$O$52, 1) +COUNTIF(O$2:O45,O45) -1</f>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -3869,8 +3870,8 @@
         <v>-3.0010420686993711E-3</v>
       </c>
       <c r="F46" s="9">
-        <f>_xlfn.RANK.EQ($E46, $E$2:$E$52) +COUNTIF(E$2:E46,E46) -1</f>
-        <v>9</v>
+        <f>_xlfn.RANK.EQ($E46, $E$2:$E$52, 1) +COUNTIF(E$2:E46,E46) -1</f>
+        <v>43</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -3886,9 +3887,9 @@
         <f t="shared" si="3"/>
         <v>-3.2319887218048821E-2</v>
       </c>
-      <c r="K46" s="10">
-        <f>_xlfn.RANK.EQ($J46, $J$2:$J$52) +COUNTIF(J$2:J46,J46) -1</f>
-        <v>19</v>
+      <c r="K46" s="9">
+        <f>_xlfn.RANK.EQ($J46, $J$2:$J$52, 1) +COUNTIF(J$2:J46,J46) -1</f>
+        <v>33</v>
       </c>
       <c r="L46">
         <v>267100</v>
@@ -3904,9 +3905,9 @@
         <f t="shared" si="5"/>
         <v>-4.6225533508053113E-2</v>
       </c>
-      <c r="P46" s="10">
-        <f>_xlfn.RANK.EQ($O46, $O$2:$O$52) +COUNTIF(O$2:O46,O46) -1</f>
-        <v>36</v>
+      <c r="P46" s="9">
+        <f>_xlfn.RANK.EQ($O46, $O$2:$O$52, 1) +COUNTIF(O$2:O46,O46) -1</f>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3928,8 +3929,8 @@
         <v>-1.7435939690898361E-4</v>
       </c>
       <c r="F47" s="9">
-        <f>_xlfn.RANK.EQ($E47, $E$2:$E$52) +COUNTIF(E$2:E47,E47) -1</f>
-        <v>7</v>
+        <f>_xlfn.RANK.EQ($E47, $E$2:$E$52, 1) +COUNTIF(E$2:E47,E47) -1</f>
+        <v>45</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -3945,9 +3946,9 @@
         <f t="shared" si="3"/>
         <v>-3.3291600310348285E-4</v>
       </c>
-      <c r="K47" s="10">
-        <f>_xlfn.RANK.EQ($J47, $J$2:$J$52) +COUNTIF(J$2:J47,J47) -1</f>
-        <v>7</v>
+      <c r="K47" s="9">
+        <f>_xlfn.RANK.EQ($J47, $J$2:$J$52, 1) +COUNTIF(J$2:J47,J47) -1</f>
+        <v>45</v>
       </c>
       <c r="L47">
         <v>75072800</v>
@@ -3963,9 +3964,9 @@
         <f t="shared" si="5"/>
         <v>-2.9266019117572752E-4</v>
       </c>
-      <c r="P47" s="10">
-        <f>_xlfn.RANK.EQ($O47, $O$2:$O$52) +COUNTIF(O$2:O47,O47) -1</f>
-        <v>14</v>
+      <c r="P47" s="9">
+        <f>_xlfn.RANK.EQ($O47, $O$2:$O$52, 1) +COUNTIF(O$2:O47,O47) -1</f>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -3987,8 +3988,8 @@
         <v>-3.1133192323107857E-2</v>
       </c>
       <c r="F48" s="9">
-        <f>_xlfn.RANK.EQ($E48, $E$2:$E$52) +COUNTIF(E$2:E48,E48) -1</f>
-        <v>32</v>
+        <f>_xlfn.RANK.EQ($E48, $E$2:$E$52, 1) +COUNTIF(E$2:E48,E48) -1</f>
+        <v>20</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -4004,9 +4005,9 @@
         <f t="shared" si="3"/>
         <v>-4.0559890224125802E-2</v>
       </c>
-      <c r="K48" s="10">
-        <f>_xlfn.RANK.EQ($J48, $J$2:$J$52) +COUNTIF(J$2:J48,J48) -1</f>
-        <v>23</v>
+      <c r="K48" s="9">
+        <f>_xlfn.RANK.EQ($J48, $J$2:$J$52, 1) +COUNTIF(J$2:J48,J48) -1</f>
+        <v>29</v>
       </c>
       <c r="L48">
         <v>7289800</v>
@@ -4022,9 +4023,9 @@
         <f t="shared" si="5"/>
         <v>-5.5893132870587676E-2</v>
       </c>
-      <c r="P48" s="10">
-        <f>_xlfn.RANK.EQ($O48, $O$2:$O$52) +COUNTIF(O$2:O48,O48) -1</f>
-        <v>37</v>
+      <c r="P48" s="9">
+        <f>_xlfn.RANK.EQ($O48, $O$2:$O$52, 1) +COUNTIF(O$2:O48,O48) -1</f>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -4046,8 +4047,8 @@
         <v>-1.8444360086767971E-2</v>
       </c>
       <c r="F49" s="9">
-        <f>_xlfn.RANK.EQ($E49, $E$2:$E$52) +COUNTIF(E$2:E49,E49) -1</f>
-        <v>25</v>
+        <f>_xlfn.RANK.EQ($E49, $E$2:$E$52, 1) +COUNTIF(E$2:E49,E49) -1</f>
+        <v>27</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -4063,9 +4064,9 @@
         <f t="shared" si="3"/>
         <v>-6.9523586744639335E-2</v>
       </c>
-      <c r="K49" s="10">
-        <f>_xlfn.RANK.EQ($J49, $J$2:$J$52) +COUNTIF(J$2:J49,J49) -1</f>
-        <v>39</v>
+      <c r="K49" s="9">
+        <f>_xlfn.RANK.EQ($J49, $J$2:$J$52, 1) +COUNTIF(J$2:J49,J49) -1</f>
+        <v>13</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -4081,9 +4082,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P49" s="10">
-        <f>_xlfn.RANK.EQ($O49, $O$2:$O$52) +COUNTIF(O$2:O49,O49) -1</f>
-        <v>3</v>
+      <c r="P49" s="9">
+        <f>_xlfn.RANK.EQ($O49, $O$2:$O$52, 1) +COUNTIF(O$2:O49,O49) -1</f>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -4105,8 +4106,8 @@
         <v>0</v>
       </c>
       <c r="F50" s="9">
-        <f>_xlfn.RANK.EQ($E50, $E$2:$E$52) +COUNTIF(E$2:E50,E50) -1</f>
-        <v>5</v>
+        <f>_xlfn.RANK.EQ($E50, $E$2:$E$52, 1) +COUNTIF(E$2:E50,E50) -1</f>
+        <v>50</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -4122,9 +4123,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K50" s="10">
-        <f>_xlfn.RANK.EQ($J50, $J$2:$J$52) +COUNTIF(J$2:J50,J50) -1</f>
-        <v>4</v>
+      <c r="K50" s="9">
+        <f>_xlfn.RANK.EQ($J50, $J$2:$J$52, 1) +COUNTIF(J$2:J50,J50) -1</f>
+        <v>51</v>
       </c>
       <c r="L50">
         <v>843200</v>
@@ -4140,9 +4141,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P50" s="10">
-        <f>_xlfn.RANK.EQ($O50, $O$2:$O$52) +COUNTIF(O$2:O50,O50) -1</f>
-        <v>4</v>
+      <c r="P50" s="9">
+        <f>_xlfn.RANK.EQ($O50, $O$2:$O$52, 1) +COUNTIF(O$2:O50,O50) -1</f>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -4164,8 +4165,8 @@
         <v>-1.2785255822058129E-2</v>
       </c>
       <c r="F51" s="9">
-        <f>_xlfn.RANK.EQ($E51, $E$2:$E$52) +COUNTIF(E$2:E51,E51) -1</f>
-        <v>17</v>
+        <f>_xlfn.RANK.EQ($E51, $E$2:$E$52, 1) +COUNTIF(E$2:E51,E51) -1</f>
+        <v>35</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -4181,9 +4182,9 @@
         <f t="shared" si="3"/>
         <v>-3.6573903982970231E-2</v>
       </c>
-      <c r="K51" s="10">
-        <f>_xlfn.RANK.EQ($J51, $J$2:$J$52) +COUNTIF(J$2:J51,J51) -1</f>
-        <v>21</v>
+      <c r="K51" s="9">
+        <f>_xlfn.RANK.EQ($J51, $J$2:$J$52, 1) +COUNTIF(J$2:J51,J51) -1</f>
+        <v>31</v>
       </c>
       <c r="L51">
         <v>8833900</v>
@@ -4199,9 +4200,9 @@
         <f t="shared" si="5"/>
         <v>-1.1100045280114048E-2</v>
       </c>
-      <c r="P51" s="10">
-        <f>_xlfn.RANK.EQ($O51, $O$2:$O$52) +COUNTIF(O$2:O51,O51) -1</f>
-        <v>19</v>
+      <c r="P51" s="9">
+        <f>_xlfn.RANK.EQ($O51, $O$2:$O$52, 1) +COUNTIF(O$2:O51,O51) -1</f>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -4223,8 +4224,8 @@
         <v>-8.009596083231342E-2</v>
       </c>
       <c r="F52" s="9">
-        <f>_xlfn.RANK.EQ($E52, $E$2:$E$52) +COUNTIF(E$2:E52,E52) -1</f>
-        <v>45</v>
+        <f>_xlfn.RANK.EQ($E52, $E$2:$E$52, 1) +COUNTIF(E$2:E52,E52) -1</f>
+        <v>7</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -4240,9 +4241,9 @@
         <f t="shared" si="3"/>
         <v>-9.6704683082722218E-2</v>
       </c>
-      <c r="K52" s="10">
-        <f>_xlfn.RANK.EQ($J52, $J$2:$J$52) +COUNTIF(J$2:J52,J52) -1</f>
-        <v>43</v>
+      <c r="K52" s="9">
+        <f>_xlfn.RANK.EQ($J52, $J$2:$J$52, 1) +COUNTIF(J$2:J52,J52) -1</f>
+        <v>9</v>
       </c>
       <c r="L52">
         <v>2321600</v>
@@ -4258,9 +4259,9 @@
         <f t="shared" si="5"/>
         <v>-0.11404408166781529</v>
       </c>
-      <c r="P52" s="10">
-        <f>_xlfn.RANK.EQ($O52, $O$2:$O$52) +COUNTIF(O$2:O52,O52) -1</f>
-        <v>46</v>
+      <c r="P52" s="9">
+        <f>_xlfn.RANK.EQ($O52, $O$2:$O$52, 1) +COUNTIF(O$2:O52,O52) -1</f>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -4653,44 +4654,44 @@
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="10">
         <f>INDEX($B$2:$B$52, MATCH($B$87, $A$2:$A$52))</f>
-        <v>409300</v>
-      </c>
-      <c r="C84">
+        <v>5249800</v>
+      </c>
+      <c r="C84" s="10">
         <f>INDEX($C$2:$C$52, MATCH($B$87, $A$2:$A$52))</f>
-        <v>385908.52</v>
+        <v>4801960.08</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="10">
         <f>INDEX($G$2:$G$52, MATCH($B$87, $A$2:$A$52))</f>
-        <v>428500</v>
-      </c>
-      <c r="C85">
+        <v>5442200</v>
+      </c>
+      <c r="C85" s="10">
         <f>INDEX($H$2:$H$52, MATCH($B$87, $A$2:$A$52))</f>
-        <v>427758.64</v>
+        <v>5122329.02999999</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="10">
         <f>INDEX($L$2:$L$52, MATCH($B$87, $A$2:$A$52))</f>
-        <v>445200</v>
-      </c>
-      <c r="C86">
+        <v>5430700</v>
+      </c>
+      <c r="C86" s="10">
         <f>INDEX($M$2:$M$52, MATCH($B$87, $A$2:$A$52))</f>
-        <v>445114.28999999899</v>
+        <v>5117235.21</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -4741,27 +4742,27 @@
       </c>
       <c r="B91" t="str">
         <f>_xlfn.XLOOKUP($B$89, $F$2:$F$52, $A$2:$A$52)</f>
-        <v>Debt Service</v>
+        <v>Clerk and Master - Chancery</v>
       </c>
       <c r="C91" s="5">
         <f>_xlfn.XLOOKUP($B91, $A$2:$A$52, $E$2:$E$52)</f>
-        <v>3.1837408866824991E-3</v>
+        <v>-0.15235918433091292</v>
       </c>
       <c r="D91" t="str">
         <f>_xlfn.XLOOKUP($D$89, $F$2:$F$52, $A$2:$A$52)</f>
-        <v>Community Oversight Board</v>
+        <v>Circuit Court Clerk</v>
       </c>
       <c r="E91" s="5">
         <f>_xlfn.XLOOKUP($D91, $A$2:$A$52, $E$2:$E$52)</f>
-        <v>0</v>
+        <v>-0.11502817362571344</v>
       </c>
       <c r="F91" t="str">
         <f>_xlfn.XLOOKUP($F$89, $F$2:$F$52, $A$2:$A$52)</f>
-        <v>Information Technology Service</v>
+        <v>Internal Audit</v>
       </c>
       <c r="G91" s="5">
         <f>_xlfn.XLOOKUP($F91, $A$2:$A$52, $E$2:$E$52)</f>
-        <v>0</v>
+        <v>-9.5782760864849215E-2</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -4770,27 +4771,27 @@
       </c>
       <c r="B92" t="str">
         <f>_xlfn.XLOOKUP($B$89, $K$2:$K$52, $A$2:$A$52)</f>
-        <v>Community Oversight Board</v>
+        <v>Metropolitan Clerk</v>
       </c>
       <c r="C92" s="5">
         <f>_xlfn.XLOOKUP($B92, $A$2:$A$52, $J$2:$J$52)</f>
-        <v>0</v>
+        <v>-0.17551246244575608</v>
       </c>
       <c r="D92" t="str">
         <f>_xlfn.XLOOKUP($D$89, $K$2:$K$52, $A$2:$A$52)</f>
-        <v>Information Technology Service</v>
+        <v>Internal Audit</v>
       </c>
       <c r="E92" s="5">
         <f t="shared" ref="E92:E93" si="12">_xlfn.XLOOKUP($D92, $A$2:$A$52, $J$2:$J$52)</f>
-        <v>0</v>
+        <v>-0.17103239309050916</v>
       </c>
       <c r="F92" t="str">
         <f>_xlfn.XLOOKUP($F$89, $K$2:$K$52, $A$2:$A$52)</f>
-        <v>Medical Examiner</v>
+        <v>Office of Family Safety</v>
       </c>
       <c r="G92" s="5">
         <f>_xlfn.XLOOKUP($F92, $A$2:$A$52, $J$2:$J$52)</f>
-        <v>0</v>
+        <v>-0.13918241656366656</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -4799,27 +4800,27 @@
       </c>
       <c r="B93" t="str">
         <f>_xlfn.XLOOKUP($B$89, $P$2:$P$52, $A$2:$A$52)</f>
-        <v>Information Technology Service</v>
+        <v>Community Oversight Board</v>
       </c>
       <c r="C93" s="5">
         <f>_xlfn.XLOOKUP($B93, $A$2:$A$52, $O$2:$O$52)</f>
-        <v>0</v>
+        <v>-0.82994157333333329</v>
       </c>
       <c r="D93" t="str">
         <f>_xlfn.XLOOKUP($D$89, $P$2:$P$52, $A$2:$A$52)</f>
-        <v>Medical Examiner</v>
+        <v>Clerk and Master - Chancery</v>
       </c>
       <c r="E93" s="5">
         <f>_xlfn.XLOOKUP($D93, $A$2:$A$52, $O$2:$O$52)</f>
-        <v>0</v>
+        <v>-0.15295680364719175</v>
       </c>
       <c r="F93" t="str">
         <f>_xlfn.XLOOKUP($F$89, $P$2:$P$52, $A$2:$A$52)</f>
-        <v>Soil and Water Conservation</v>
+        <v>Election Commission</v>
       </c>
       <c r="G93" s="5">
         <f t="shared" ref="G92:G93" si="13">_xlfn.XLOOKUP($F93, $A$2:$A$52, $O$2:$O$52)</f>
-        <v>0</v>
+        <v>-0.12882667147667154</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -4869,27 +4870,27 @@
       </c>
       <c r="B98" t="str">
         <f>INDEX($A$2:$P$52, MATCH($B$96, $F$2:$F$52, 0), 1)</f>
-        <v>Debt Service</v>
+        <v>Clerk and Master - Chancery</v>
       </c>
       <c r="C98" s="5">
         <f>INDEX($A$2:$P$52, MATCH($B98, $A$2:$A$52, 0), 5)</f>
-        <v>3.1837408866824991E-3</v>
+        <v>-0.15235918433091292</v>
       </c>
       <c r="D98" t="str">
         <f>INDEX($A$2:$P$52, MATCH($D$96, $F$2:$F$52, 0), 1)</f>
-        <v>Community Oversight Board</v>
+        <v>Circuit Court Clerk</v>
       </c>
       <c r="E98" s="4">
         <f>INDEX($A$2:$P$52, MATCH($D98, $A$2:$A$52, 0), 5)</f>
-        <v>0</v>
+        <v>-0.11502817362571344</v>
       </c>
       <c r="F98" t="str">
         <f>INDEX($A$2:$P$52, MATCH($F$96, $F$2:$F$52, 0), 1)</f>
-        <v>Information Technology Service</v>
+        <v>Internal Audit</v>
       </c>
       <c r="G98" s="4">
         <f>INDEX($A$2:$P$52, MATCH($F98, $A$2:$A$52, 0), 5)</f>
-        <v>0</v>
+        <v>-9.5782760864849215E-2</v>
       </c>
       <c r="I98" s="4"/>
     </row>
@@ -4899,27 +4900,27 @@
       </c>
       <c r="B99" t="str">
         <f>INDEX($A$2:$P$52, MATCH($B$96, $K$2:$K$52, 0), 1)</f>
-        <v>Community Oversight Board</v>
+        <v>Metropolitan Clerk</v>
       </c>
       <c r="C99" s="5">
         <f>INDEX($A$2:$P$52, MATCH($B99, $A$2:$A$52, 0), 10)</f>
-        <v>0</v>
+        <v>-0.17551246244575608</v>
       </c>
       <c r="D99" t="str">
         <f>INDEX($A$2:$P$52, MATCH($D$96, $K$2:$K$52, 0), 1)</f>
-        <v>Information Technology Service</v>
+        <v>Internal Audit</v>
       </c>
       <c r="E99" s="4">
         <f>INDEX($A$2:$P$52, MATCH($D99, $A$2:$A$52, 0), 10)</f>
-        <v>0</v>
+        <v>-0.17103239309050916</v>
       </c>
       <c r="F99" t="str">
         <f>INDEX($A$2:$P$52, MATCH($F$96, $K$2:$K$52, 0), 1)</f>
-        <v>Medical Examiner</v>
+        <v>Office of Family Safety</v>
       </c>
       <c r="G99" s="4">
         <f>INDEX($A$2:$P$52, MATCH($F99, $A$2:$A$52, 0), 10)</f>
-        <v>0</v>
+        <v>-0.13918241656366656</v>
       </c>
       <c r="I99" s="4"/>
     </row>
@@ -4929,33 +4930,33 @@
       </c>
       <c r="B100" t="str">
         <f>INDEX($A$2:$P$52, MATCH($B$96, $P$2:$P$52, 0), 1)</f>
-        <v>Information Technology Service</v>
+        <v>Community Oversight Board</v>
       </c>
       <c r="C100" s="5">
         <f>INDEX($A$2:$P$52, MATCH($B100, $A$2:$A$52, 0), 15)</f>
-        <v>0</v>
+        <v>-0.82994157333333329</v>
       </c>
       <c r="D100" t="str">
         <f>INDEX($A$2:$P$52, MATCH($D$96, $P$2:$P$52, 0), 1)</f>
-        <v>Medical Examiner</v>
+        <v>Clerk and Master - Chancery</v>
       </c>
       <c r="E100" s="4">
         <f>INDEX($A$2:$P$52, MATCH($D100, $A$2:$A$52, 0), 15)</f>
-        <v>0</v>
+        <v>-0.15295680364719175</v>
       </c>
       <c r="F100" t="str">
         <f>INDEX($A$2:$P$52, MATCH($F$96, $P$2:$P$52, 0), 1)</f>
-        <v>Soil and Water Conservation</v>
+        <v>Election Commission</v>
       </c>
       <c r="G100" s="4">
         <f>INDEX($A$2:$P$52, MATCH($F100, $A$2:$A$52, 0), 15)</f>
-        <v>0</v>
+        <v>-0.12882667147667154</v>
       </c>
       <c r="I100" s="4"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83 B87" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>

</xml_diff>